<commit_message>
Updated benchmarks. Latest andengine.jar .
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="17715" windowHeight="7740"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="17715" windowHeight="7740" tabRatio="889"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="61">
   <si>
     <t>TickerText</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Box2D-Physics</t>
-  </si>
-  <si>
-    <t>1.5</t>
   </si>
   <si>
     <t>VanillaEclair 4.0</t>
@@ -152,9 +149,6 @@
     <t>Tattoo (1.6)</t>
   </si>
   <si>
-    <t>Hero (1.5)</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
     <t>Magic/myTouch 3G (1.6)</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Android-Version</t>
   </si>
   <si>
@@ -202,12 +193,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Tests-Samples</t>
+  </si>
+  <si>
+    <t>Dream / G1  (Cyanogen 2.1)</t>
+  </si>
+  <si>
+    <t>Cyanogen 2.1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,19 +277,30 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -306,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -483,19 +494,6 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -554,77 +552,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -652,23 +585,67 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
         <color indexed="64"/>
-      </bottom>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -693,9 +670,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -738,11 +712,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -761,28 +732,13 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -791,26 +747,53 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="70"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="70"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="70"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="283">
+  <dxfs count="288">
     <dxf>
       <font>
         <b/>
@@ -1916,16 +1899,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -1963,16 +1936,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2010,16 +1973,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2057,16 +2010,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2104,16 +2047,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2151,16 +2084,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -2200,16 +2123,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -2255,35 +2168,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -3961,6 +3845,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -3998,6 +3892,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -4035,6 +3939,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -4072,6 +3986,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -4109,6 +4033,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -4146,6 +4080,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -4185,6 +4129,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -4230,6 +4184,35 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
@@ -5511,6 +5494,24 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -5578,7 +5579,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -5609,7 +5610,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5640,7 +5641,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5671,7 +5672,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5702,7 +5703,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5733,7 +5734,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5764,7 +5765,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -5778,9 +5779,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5831,11 +5829,13 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -5865,7 +5865,7 @@
       </font>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5896,7 +5896,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -5927,7 +5927,7 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -6083,20 +6083,20 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium16 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="282"/>
-      <tableStyleElement type="headerRow" dxfId="281"/>
-      <tableStyleElement type="totalRow" dxfId="280"/>
-      <tableStyleElement type="firstColumn" dxfId="279"/>
-      <tableStyleElement type="lastColumn" dxfId="278"/>
-      <tableStyleElement type="firstRowStripe" dxfId="277"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="276"/>
+      <tableStyleElement type="wholeTable" dxfId="287"/>
+      <tableStyleElement type="headerRow" dxfId="286"/>
+      <tableStyleElement type="totalRow" dxfId="285"/>
+      <tableStyleElement type="firstColumn" dxfId="284"/>
+      <tableStyleElement type="lastColumn" dxfId="283"/>
+      <tableStyleElement type="firstRowStripe" dxfId="282"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="281"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Benchmark" displayName="Benchmark" ref="B4:M21" headerRowDxfId="275" dataDxfId="273" totalsRowDxfId="272" headerRowBorderDxfId="274">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Benchmark" displayName="Benchmark" ref="B4:M21" headerRowDxfId="280" dataDxfId="278" totalsRowDxfId="277" headerRowBorderDxfId="279">
   <autoFilter ref="B4:M21">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -6108,22 +6108,22 @@
     <sortCondition descending="1" ref="M4:M21"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" name="Manufacturer" totalsRowLabel="Ergebnis" dataDxfId="271" totalsRowDxfId="270"/>
-    <tableColumn id="9" name="Model" dataDxfId="269" totalsRowDxfId="268"/>
-    <tableColumn id="8" name="Android-Version" dataDxfId="267" totalsRowDxfId="266"/>
-    <tableColumn id="11" name="CPU-Clock (MHz)" dataDxfId="265" totalsRowDxfId="264"/>
-    <tableColumn id="12" name="Tests" dataDxfId="263" totalsRowDxfId="262">
+    <tableColumn id="1" name="Manufacturer" totalsRowLabel="Ergebnis" dataDxfId="276" totalsRowDxfId="275"/>
+    <tableColumn id="9" name="Model" dataDxfId="274" totalsRowDxfId="273"/>
+    <tableColumn id="8" name="Android-Version" dataDxfId="272" totalsRowDxfId="271"/>
+    <tableColumn id="11" name="CPU-Clock (MHz)" dataDxfId="270" totalsRowDxfId="269"/>
+    <tableColumn id="12" name="Tests-Samples" dataDxfId="268">
       <calculatedColumnFormula>SUBTOTAL(2,Samsung_Galaxy_S_2.1[])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Sprite" totalsRowFunction="average" dataDxfId="261" totalsRowDxfId="260">
-      <calculatedColumnFormula>SUBTOTAL(101,HTC_Hero_1.5[Sprite])</calculatedColumnFormula>
+    <tableColumn id="2" name="Sprite" totalsRowFunction="average" dataDxfId="267" totalsRowDxfId="266">
+      <calculatedColumnFormula>SUBTOTAL(101,#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Animation" totalsRowFunction="average" dataDxfId="259" totalsRowDxfId="258"/>
-    <tableColumn id="4" name="ShapeModifier" totalsRowFunction="average" dataDxfId="257" totalsRowDxfId="256"/>
-    <tableColumn id="5" name="TickerText" totalsRowFunction="average" dataDxfId="255" totalsRowDxfId="254"/>
-    <tableColumn id="6" name="ParticleSystem" totalsRowFunction="sum" dataDxfId="253" totalsRowDxfId="252"/>
-    <tableColumn id="7" name="Box2D-Physics" totalsRowFunction="sum" dataDxfId="251" totalsRowDxfId="250"/>
-    <tableColumn id="10" name="Average" totalsRowFunction="average" dataDxfId="249" totalsRowDxfId="248">
+    <tableColumn id="3" name="Animation" totalsRowFunction="average" dataDxfId="265" totalsRowDxfId="264"/>
+    <tableColumn id="4" name="ShapeModifier" totalsRowFunction="average" dataDxfId="263" totalsRowDxfId="262"/>
+    <tableColumn id="5" name="TickerText" totalsRowFunction="average" dataDxfId="261" totalsRowDxfId="260"/>
+    <tableColumn id="6" name="ParticleSystem" totalsRowFunction="sum" dataDxfId="259" totalsRowDxfId="258"/>
+    <tableColumn id="7" name="Box2D-Physics" totalsRowFunction="sum" dataDxfId="257" totalsRowDxfId="256"/>
+    <tableColumn id="10" name="Average" totalsRowFunction="average" dataDxfId="255" totalsRowDxfId="254">
       <calculatedColumnFormula>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -6132,37 +6132,37 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="HTC_Droid_Incredible_2.1" displayName="HTC_Droid_Incredible_2.1" ref="A49:G49" headerRowCount="0" totalsRowShown="0" headerRowDxfId="122" dataDxfId="120" headerRowBorderDxfId="121" tableBorderDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="HTC_Evo_4G_Supersonic_2.1" displayName="HTC_Evo_4G_Supersonic_2.1" ref="A54:G54" headerRowCount="0" totalsRowShown="0" headerRowDxfId="121" dataDxfId="119" headerRowBorderDxfId="120" tableBorderDxfId="118">
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" headerRowDxfId="118" dataDxfId="117"/>
-    <tableColumn id="1" name="Sprite" headerRowDxfId="116" dataDxfId="115"/>
-    <tableColumn id="2" name="Animation" headerRowDxfId="114" dataDxfId="113"/>
-    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="112" dataDxfId="111"/>
-    <tableColumn id="4" name="TickerText" headerRowDxfId="110" dataDxfId="109"/>
-    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="108" dataDxfId="107"/>
-    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="106" dataDxfId="105"/>
+    <tableColumn id="7" name="Test-Version" headerRowDxfId="117" dataDxfId="116"/>
+    <tableColumn id="1" name="Sprite" headerRowDxfId="115" dataDxfId="114"/>
+    <tableColumn id="2" name="Animation" headerRowDxfId="113" dataDxfId="112"/>
+    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="111" dataDxfId="110"/>
+    <tableColumn id="4" name="TickerText" headerRowDxfId="109" dataDxfId="108"/>
+    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="107" dataDxfId="106"/>
+    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="105" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="HTC_Evo_4G_Supersonic_2.1" displayName="HTC_Evo_4G_Supersonic_2.1" ref="A52:G52" headerRowCount="0" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="HTC_Desire_2.1" displayName="HTC_Desire_2.1" ref="A41:G41" headerRowCount="0" totalsRowShown="0" headerRowDxfId="103" dataDxfId="101" headerRowBorderDxfId="102" tableBorderDxfId="100">
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" headerRowDxfId="100" dataDxfId="99"/>
-    <tableColumn id="1" name="Sprite" headerRowDxfId="98" dataDxfId="97"/>
-    <tableColumn id="2" name="Animation" headerRowDxfId="96" dataDxfId="95"/>
-    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="94" dataDxfId="93"/>
-    <tableColumn id="4" name="TickerText" headerRowDxfId="92" dataDxfId="91"/>
-    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="90" dataDxfId="89"/>
-    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="88" dataDxfId="87"/>
+    <tableColumn id="7" name="Test-Version" headerRowDxfId="99" dataDxfId="98"/>
+    <tableColumn id="1" name="Sprite" headerRowDxfId="97" dataDxfId="96"/>
+    <tableColumn id="2" name="Animation" headerRowDxfId="95" dataDxfId="94"/>
+    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="93" dataDxfId="92"/>
+    <tableColumn id="4" name="TickerText" headerRowDxfId="91" dataDxfId="90"/>
+    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="89" dataDxfId="88"/>
+    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="87" dataDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="HTC_Desire_2.1" displayName="HTC_Desire_2.1" ref="A40:G40" headerRowCount="0" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="HTC_Nexus_One_2.2_MoDaCo_r20" displayName="HTC_Nexus_One_2.2_MoDaCo_r20" ref="A38:G38" headerRowCount="0" totalsRowShown="0" headerRowDxfId="85" headerRowBorderDxfId="84" tableBorderDxfId="83">
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="82" dataDxfId="81"/>
     <tableColumn id="1" name="Sprite" headerRowDxfId="80" dataDxfId="79"/>
@@ -6177,7 +6177,7 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="HTC_Nexus_One_2.2_MoDaCo_r20" displayName="HTC_Nexus_One_2.2_MoDaCo_r20" ref="A37:G37" headerRowCount="0" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="HTC_Hero_Hiapk_2.18" displayName="HTC_Hero_Hiapk_2.18" ref="A7:G7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="65" dataDxfId="64"/>
     <tableColumn id="1" name="Sprite" headerRowDxfId="63" dataDxfId="62"/>
@@ -6192,7 +6192,10 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="HTC_Hero_Hiapk_2.18" displayName="HTC_Hero_Hiapk_2.18" ref="A10:G10" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="HTC_Dream_Cyanogen_2.1" displayName="HTC_Dream_Cyanogen_2.1" ref="A21:G21" headerRowCount="0" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
+  <sortState ref="A21:G24">
+    <sortCondition descending="1" ref="A15"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="48" dataDxfId="47"/>
     <tableColumn id="1" name="Sprite" headerRowDxfId="46" dataDxfId="45"/>
@@ -6223,8 +6226,8 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Motorola_Droid_2.1" displayName="Motorola_Droid_2.1" ref="A3:G8" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
-  <autoFilter ref="A3:G8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Motorola_Droid_2.1" displayName="Motorola_Droid_2.1" ref="A3:G9" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="23" tableBorderDxfId="22">
+  <autoFilter ref="A3:G9">
     <filterColumn colId="0">
       <filters>
         <filter val="1.1.1"/>
@@ -6281,23 +6284,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="HTC_Hero_1.5" displayName="HTC_Hero_1.5" ref="A3:G4" totalsRowShown="0" headerRowDxfId="247" headerRowBorderDxfId="246" tableBorderDxfId="245">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HTC_Hero_VanillaEclair_4.0" displayName="HTC_Hero_VanillaEclair_4.0" ref="A3:G4" totalsRowShown="0" headerRowDxfId="253" headerRowBorderDxfId="252" tableBorderDxfId="251">
   <autoFilter ref="A3:G4"/>
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" dataDxfId="244"/>
-    <tableColumn id="1" name="Sprite"/>
-    <tableColumn id="2" name="Animation"/>
-    <tableColumn id="3" name="ShapeModifier"/>
-    <tableColumn id="4" name="TickerText"/>
-    <tableColumn id="5" name="ParticleSystem"/>
-    <tableColumn id="6" name="Box2D-Physics"/>
+    <tableColumn id="7" name="Test-Version" dataDxfId="250"/>
+    <tableColumn id="1" name="Sprite" dataDxfId="249"/>
+    <tableColumn id="2" name="Animation" dataDxfId="248"/>
+    <tableColumn id="3" name="ShapeModifier" dataDxfId="247"/>
+    <tableColumn id="4" name="TickerText" dataDxfId="246"/>
+    <tableColumn id="5" name="ParticleSystem" dataDxfId="245"/>
+    <tableColumn id="6" name="Box2D-Physics" dataDxfId="244"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="HTC_Hero_VanillaEclair_4.0" displayName="HTC_Hero_VanillaEclair_4.0" ref="A7:G7" headerRowCount="0" totalsRowShown="0" headerRowDxfId="243" headerRowBorderDxfId="242" tableBorderDxfId="241">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="HTC_Tattoo_1.6" displayName="HTC_Tattoo_1.6" ref="A10:G12" headerRowCount="0" totalsRowShown="0" headerRowDxfId="243" headerRowBorderDxfId="242" tableBorderDxfId="241">
+  <sortState ref="A10:G12">
+    <sortCondition descending="1" ref="A10"/>
+  </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="240" dataDxfId="239"/>
     <tableColumn id="1" name="Sprite" headerRowDxfId="238" dataDxfId="237"/>
@@ -6312,9 +6318,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="HTC_Tattoo_1.6" displayName="HTC_Tattoo_1.6" ref="A13:G15" headerRowCount="0" totalsRowShown="0" headerRowDxfId="226" headerRowBorderDxfId="225" tableBorderDxfId="224">
-  <sortState ref="A10:G12">
-    <sortCondition descending="1" ref="A10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="HTC_Dream_1.6" displayName="HTC_Dream_1.6" ref="A15:G18" headerRowCount="0" totalsRowShown="0" headerRowDxfId="226" headerRowBorderDxfId="225" tableBorderDxfId="224">
+  <sortState ref="A15:G18">
+    <sortCondition descending="1" ref="A15"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="223" dataDxfId="222"/>
@@ -6330,9 +6336,9 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="HTC_Dream_1.6" displayName="HTC_Dream_1.6" ref="A18:G21" headerRowCount="0" totalsRowShown="0" headerRowDxfId="209" headerRowBorderDxfId="208" tableBorderDxfId="207">
-  <sortState ref="A15:G18">
-    <sortCondition descending="1" ref="A15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HTC_Nexus_One_2.1" displayName="HTC_Nexus_One_2.1" ref="A24:G27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="209" headerRowBorderDxfId="208" tableBorderDxfId="207">
+  <sortState ref="A21:G24">
+    <sortCondition descending="1" ref="A21"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="206" dataDxfId="205"/>
@@ -6348,9 +6354,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="HTC_Nexus_One_2.1" displayName="HTC_Nexus_One_2.1" ref="A24:G27" headerRowCount="0" totalsRowShown="0" headerRowDxfId="192" headerRowBorderDxfId="191" tableBorderDxfId="190">
-  <sortState ref="A21:G24">
-    <sortCondition descending="1" ref="A21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="HTC_Nexus_One_2.2" displayName="HTC_Nexus_One_2.2" ref="A30:G35" headerRowCount="0" totalsRowShown="0" headerRowDxfId="192" headerRowBorderDxfId="191" tableBorderDxfId="190">
+  <sortState ref="A27:G30">
+    <sortCondition descending="1" ref="A27"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="7" name="Test-Version" headerRowDxfId="189" dataDxfId="188"/>
@@ -6366,48 +6372,45 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="HTC_Nexus_One_2.2" displayName="HTC_Nexus_One_2.2" ref="A30:G34" headerRowCount="0" totalsRowShown="0" headerRowDxfId="175" headerRowBorderDxfId="174" tableBorderDxfId="173">
-  <sortState ref="A27:G30">
-    <sortCondition descending="1" ref="A27"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="HTC_Legend_2.1" displayName="HTC_Legend_2.1" ref="A44:G44" headerRowCount="0" totalsRowShown="0" headerRowDxfId="175" dataDxfId="173" headerRowBorderDxfId="174" tableBorderDxfId="172">
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" headerRowDxfId="172" dataDxfId="171"/>
-    <tableColumn id="1" name="Sprite" headerRowDxfId="170" dataDxfId="169"/>
-    <tableColumn id="2" name="Animation" headerRowDxfId="168" dataDxfId="167"/>
-    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="166" dataDxfId="165"/>
-    <tableColumn id="4" name="TickerText" headerRowDxfId="164" dataDxfId="163"/>
-    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="162" dataDxfId="161"/>
-    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="160" dataDxfId="159"/>
+    <tableColumn id="7" name="Test-Version" headerRowDxfId="171" dataDxfId="170"/>
+    <tableColumn id="1" name="Sprite" headerRowDxfId="169" dataDxfId="168"/>
+    <tableColumn id="2" name="Animation" headerRowDxfId="167" dataDxfId="166"/>
+    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="165" dataDxfId="164"/>
+    <tableColumn id="4" name="TickerText" headerRowDxfId="163" dataDxfId="162"/>
+    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="161" dataDxfId="160"/>
+    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="159" dataDxfId="158"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="HTC_Legend_2.1" displayName="HTC_Legend_2.1" ref="A43:G43" headerRowCount="0" totalsRowShown="0" headerRowDxfId="158" dataDxfId="156" headerRowBorderDxfId="157" tableBorderDxfId="155">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="HTC_myTouch3G_1.6" displayName="HTC_myTouch3G_1.6" ref="A47:G48" headerRowCount="0" totalsRowShown="0" headerRowDxfId="157" dataDxfId="155" headerRowBorderDxfId="156" tableBorderDxfId="154">
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" headerRowDxfId="154" dataDxfId="153"/>
-    <tableColumn id="1" name="Sprite" headerRowDxfId="152" dataDxfId="151"/>
-    <tableColumn id="2" name="Animation" headerRowDxfId="150" dataDxfId="149"/>
-    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="148" dataDxfId="147"/>
-    <tableColumn id="4" name="TickerText" headerRowDxfId="146" dataDxfId="145"/>
-    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="144" dataDxfId="143"/>
-    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="142" dataDxfId="141"/>
+    <tableColumn id="7" name="Test-Version" headerRowDxfId="153" dataDxfId="152"/>
+    <tableColumn id="1" name="Sprite" headerRowDxfId="151" dataDxfId="150"/>
+    <tableColumn id="2" name="Animation" headerRowDxfId="149" dataDxfId="148"/>
+    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="147" dataDxfId="146"/>
+    <tableColumn id="4" name="TickerText" headerRowDxfId="145" dataDxfId="144"/>
+    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="143" dataDxfId="142"/>
+    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="141" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="HTC_myTouch3G_1.6" displayName="HTC_myTouch3G_1.6" ref="A46:G46" headerRowCount="0" totalsRowShown="0" headerRowDxfId="140" dataDxfId="138" headerRowBorderDxfId="139" tableBorderDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="HTC_Droid_Incredible_2.1" displayName="HTC_Droid_Incredible_2.1" ref="A51:G51" headerRowCount="0" totalsRowShown="0" headerRowDxfId="139" dataDxfId="137" headerRowBorderDxfId="138" tableBorderDxfId="136">
   <tableColumns count="7">
-    <tableColumn id="7" name="Test-Version" headerRowDxfId="136" dataDxfId="135"/>
-    <tableColumn id="1" name="Sprite" headerRowDxfId="134" dataDxfId="133"/>
-    <tableColumn id="2" name="Animation" headerRowDxfId="132" dataDxfId="131"/>
-    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="130" dataDxfId="129"/>
-    <tableColumn id="4" name="TickerText" headerRowDxfId="128" dataDxfId="127"/>
-    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="126" dataDxfId="125"/>
-    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="124" dataDxfId="123"/>
+    <tableColumn id="7" name="Test-Version" headerRowDxfId="135" dataDxfId="134"/>
+    <tableColumn id="1" name="Sprite" headerRowDxfId="133" dataDxfId="132"/>
+    <tableColumn id="2" name="Animation" headerRowDxfId="131" dataDxfId="130"/>
+    <tableColumn id="3" name="ShapeModifier" headerRowDxfId="129" dataDxfId="128"/>
+    <tableColumn id="4" name="TickerText" headerRowDxfId="127" dataDxfId="126"/>
+    <tableColumn id="5" name="ParticleSystem" headerRowDxfId="125" dataDxfId="124"/>
+    <tableColumn id="6" name="Box2D-Physics" headerRowDxfId="123" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6703,847 +6706,847 @@
   </sheetPr>
   <dimension ref="B2:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" customWidth="1"/>
     <col min="7" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="23.25">
-      <c r="F2" s="30" t="s">
-        <v>51</v>
+      <c r="G2" s="29" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:14" ht="75" customHeight="1" thickBot="1">
-      <c r="B4" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="54" t="s">
+      <c r="C4" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="56" t="s">
+      <c r="J4" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="K4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="57" t="s">
+      <c r="L4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="58" t="s">
-        <v>45</v>
+      <c r="M4" s="44" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="49">
-        <v>528</v>
-      </c>
-      <c r="F5" s="46">
-        <f>SUBTOTAL(2,HTC_Hero_1.5[])</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="43" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[Sprite])),"?",(SUBTOTAL(1,HTC_Hero_1.5[Sprite])))</f>
-        <v>?</v>
-      </c>
-      <c r="H5" s="44" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[Animation])),"?",(SUBTOTAL(1,HTC_Hero_1.5[Animation])))</f>
-        <v>?</v>
-      </c>
-      <c r="I5" s="44" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Hero_1.5[ShapeModifier])))</f>
-        <v>?</v>
-      </c>
-      <c r="J5" s="44" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[TickerText])),"?",(SUBTOTAL(1,HTC_Hero_1.5[TickerText])))</f>
-        <v>?</v>
-      </c>
-      <c r="K5" s="44" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Hero_1.5[ParticleSystem])))</f>
-        <v>?</v>
-      </c>
-      <c r="L5" s="45" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_1.5[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Hero_1.5[Box2D-Physics])))</f>
-        <v>?</v>
-      </c>
-      <c r="M5" s="31" t="str">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>?</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14">
-      <c r="B6" s="22" t="s">
+      <c r="B5" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="40">
+      <c r="D5" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="46">
         <v>1000</v>
       </c>
-      <c r="F6" s="47">
-        <f>SUBTOTAL(2,Samsung_Galaxy_S_2.1[])</f>
-        <v>6</v>
-      </c>
-      <c r="G6" s="24">
+      <c r="F5" s="47">
+        <f>SUBTOTAL(2,Samsung_Galaxy_S_2.1[])/6</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="56">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Sprite])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Sprite])))</f>
         <v>25.367393</v>
       </c>
-      <c r="H6" s="25">
+      <c r="H5" s="57">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Animation])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Animation])))</f>
         <v>28.268608</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I5" s="57">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[ShapeModifier])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[ShapeModifier])))</f>
         <v>35.899982000000001</v>
       </c>
-      <c r="J6" s="25">
+      <c r="J5" s="57">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[TickerText])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[TickerText])))</f>
         <v>25.116581</v>
       </c>
-      <c r="K6" s="25">
+      <c r="K5" s="57">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[ParticleSystem])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[ParticleSystem])))</f>
         <v>40.272410000000001</v>
       </c>
-      <c r="L6" s="34">
+      <c r="L5" s="58">
         <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,Samsung_Galaxy_S_2.1[Box2D-Physics])))</f>
         <v>31.072804999999999</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M5" s="51">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>30.99962983333333</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
-      <c r="B7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="23" t="s">
+    <row r="6" spans="2:14">
+      <c r="B6" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="40">
+      <c r="E6" s="36">
         <v>1000</v>
       </c>
-      <c r="F7" s="47">
-        <f>SUBTOTAL(2,HTC_Nexus_One_2.2[])</f>
-        <v>14</v>
-      </c>
-      <c r="G7" s="24">
+      <c r="F6" s="47">
+        <f>SUBTOTAL(2,HTC_Nexus_One_2.2[])/6</f>
+        <v>2.5</v>
+      </c>
+      <c r="G6" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[Sprite])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[Sprite])))</f>
-        <v>14.798061666666667</v>
-      </c>
-      <c r="H7" s="25">
+        <v>14.922869500000001</v>
+      </c>
+      <c r="H6" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[Animation])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[Animation])))</f>
         <v>16.313920500000002</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I6" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[ShapeModifier])))</f>
         <v>19.314080999999998</v>
       </c>
-      <c r="J7" s="25">
+      <c r="J6" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[TickerText])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[TickerText])))</f>
         <v>18.939761000000001</v>
       </c>
-      <c r="K7" s="25">
+      <c r="K6" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[ParticleSystem])))</f>
         <v>25.525525999999999</v>
       </c>
-      <c r="L7" s="34">
+      <c r="L6" s="30">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2[Box2D-Physics])))</f>
         <v>24.2664303</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M6" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>19.859630077777776</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="40">
+        <v>19.880431383333335</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="36">
         <v>1000</v>
       </c>
-      <c r="F8" s="47">
-        <f>SUBTOTAL(2,HTC_Nexus_One_2.2_MoDaCo_r20[])</f>
-        <v>6</v>
-      </c>
-      <c r="G8" s="24">
+      <c r="F7" s="47">
+        <f>SUBTOTAL(2,HTC_Nexus_One_2.2_MoDaCo_r20[])/6</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Sprite])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Sprite])))</f>
         <v>17.269221999999999</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H7" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Animation])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Animation])))</f>
         <v>15.531084999999999</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I7" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[ShapeModifier])))</f>
         <v>18.836193000000002</v>
       </c>
-      <c r="J8" s="25">
+      <c r="J7" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[TickerText])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[TickerText])))</f>
         <v>17.784476999999999</v>
       </c>
-      <c r="K8" s="25">
+      <c r="K7" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[ParticleSystem])))</f>
         <v>21.471651000000001</v>
       </c>
-      <c r="L8" s="34">
+      <c r="L7" s="30">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.2_MoDaCo_r20[Box2D-Physics])))</f>
         <v>20.804794000000001</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M7" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>18.616237000000002</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="22" t="s">
+    <row r="8" spans="2:14">
+      <c r="B8" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="40">
-        <v>550</v>
-      </c>
-      <c r="F9" s="47">
-        <f>SUBTOTAL(2,Motorola_Droid_2.1[])</f>
-        <v>4</v>
-      </c>
-      <c r="G9" s="24" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Sprite])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Sprite])))</f>
-        <v>?</v>
-      </c>
-      <c r="H9" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Animation])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Animation])))</f>
-        <v>?</v>
-      </c>
-      <c r="I9" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[ShapeModifier])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[ShapeModifier])))</f>
-        <v>20.46621</v>
-      </c>
-      <c r="J9" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[TickerText])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[TickerText])))</f>
-        <v>7.0465616999999998</v>
-      </c>
-      <c r="K9" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[ParticleSystem])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[ParticleSystem])))</f>
-        <v>15.621314</v>
-      </c>
-      <c r="L9" s="34">
-        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Box2D-Physics])))</f>
-        <v>15.525149000000001</v>
-      </c>
-      <c r="M9" s="32">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>14.664808675</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="40">
+      <c r="E8" s="36">
         <v>1000</v>
       </c>
-      <c r="F10" s="47">
-        <f>SUBTOTAL(2,HTC_Droid_Incredible_2.1[])</f>
-        <v>5</v>
-      </c>
-      <c r="G10" s="24">
+      <c r="F8" s="47">
+        <f>SUBTOTAL(2,HTC_Droid_Incredible_2.1[])/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G8" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[Sprite])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[Sprite])))</f>
         <v>13.379421000000001</v>
       </c>
-      <c r="H10" s="25">
+      <c r="H8" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[Animation])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[Animation])))</f>
         <v>11.917116999999999</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I8" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[ShapeModifier])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[ShapeModifier])))</f>
         <v>15.435746999999999</v>
       </c>
-      <c r="J10" s="25">
+      <c r="J8" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[TickerText])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[TickerText])))</f>
         <v>15.865864999999999</v>
       </c>
-      <c r="K10" s="25">
+      <c r="K8" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[ParticleSystem])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[ParticleSystem])))</f>
         <v>15.810184</v>
       </c>
-      <c r="L10" s="34" t="str">
+      <c r="L8" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Droid_Incredible_2.1[Box2D-Physics])),"?",(SUBTOTAL(101,HTC_Droid_Incredible_2.1[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M8" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>14.481666799999999</v>
       </c>
-      <c r="N10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="40">
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="36">
         <v>1000</v>
       </c>
-      <c r="F11" s="47">
-        <f>SUBTOTAL(2,HTC_Desire_2.1[])</f>
-        <v>3</v>
-      </c>
-      <c r="G11" s="24" t="str">
+      <c r="F9" s="47">
+        <f>SUBTOTAL(2,HTC_Desire_2.1[])/6</f>
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="23" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[Sprite])),"?",(SUBTOTAL(1,HTC_Desire_2.1[Sprite])))</f>
         <v>?</v>
       </c>
-      <c r="H11" s="25">
+      <c r="H9" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[Animation])),"?",(SUBTOTAL(1,HTC_Desire_2.1[Animation])))</f>
         <v>11.735962000000001</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I9" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Desire_2.1[ShapeModifier])))</f>
         <v>15.083520999999999</v>
       </c>
-      <c r="J11" s="25" t="str">
+      <c r="J9" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[TickerText])),"?",(SUBTOTAL(1,HTC_Desire_2.1[TickerText])))</f>
         <v>?</v>
       </c>
-      <c r="K11" s="25">
+      <c r="K9" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Desire_2.1[ParticleSystem])))</f>
         <v>15.923451999999999</v>
       </c>
-      <c r="L11" s="34" t="str">
+      <c r="L9" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Desire_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Desire_2.1[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M9" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>14.247644999999999</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="40">
+    <row r="10" spans="2:14">
+      <c r="B10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="36">
         <v>1000</v>
       </c>
-      <c r="F12" s="47">
-        <f>SUBTOTAL(2,HTC_Nexus_One_2.1[])</f>
-        <v>11</v>
-      </c>
-      <c r="G12" s="24">
+      <c r="F10" s="47">
+        <f>SUBTOTAL(2,HTC_Nexus_One_2.1[])/6</f>
+        <v>1.8333333333333333</v>
+      </c>
+      <c r="G10" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[Sprite])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[Sprite])))</f>
         <v>14.475951250000001</v>
       </c>
-      <c r="H12" s="25">
+      <c r="H10" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[Animation])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[Animation])))</f>
         <v>11.497117699999999</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I10" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[ShapeModifier])))</f>
         <v>15.965774333333334</v>
       </c>
-      <c r="J12" s="25">
+      <c r="J10" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[TickerText])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[TickerText])))</f>
         <v>14.288466</v>
       </c>
-      <c r="K12" s="25" t="str">
+      <c r="K10" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[ParticleSystem])))</f>
         <v>?</v>
       </c>
-      <c r="L12" s="34" t="str">
+      <c r="L10" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Nexus_One_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Nexus_One_2.1[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M12" s="32">
+      <c r="M10" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>14.056827320833333</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="40">
+      <c r="N10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="36">
         <v>600</v>
       </c>
-      <c r="F13" s="47">
-        <f>SUBTOTAL(2,HTC_Legend_2.1[])</f>
-        <v>3</v>
-      </c>
-      <c r="G13" s="24" t="str">
+      <c r="F11" s="47">
+        <f>SUBTOTAL(2,HTC_Legend_2.1[])/6</f>
+        <v>0.5</v>
+      </c>
+      <c r="G11" s="23" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[Sprite])),"?",(SUBTOTAL(1,HTC_Legend_2.1[Sprite])))</f>
         <v>?</v>
       </c>
-      <c r="H13" s="25" t="str">
+      <c r="H11" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[Animation])),"?",(SUBTOTAL(1,HTC_Legend_2.1[Animation])))</f>
         <v>?</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I11" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Legend_2.1[ShapeModifier])))</f>
         <v>9.7283609999999996</v>
       </c>
-      <c r="J13" s="25">
+      <c r="J11" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[TickerText])),"?",(SUBTOTAL(1,HTC_Legend_2.1[TickerText])))</f>
         <v>21.894788999999999</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K11" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Legend_2.1[ParticleSystem])))</f>
         <v>10.11773</v>
       </c>
-      <c r="L13" s="34" t="str">
+      <c r="L11" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Legend_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Legend_2.1[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M13" s="32">
+      <c r="M11" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>13.913626666666666</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
-      <c r="B14" s="22" t="s">
+    <row r="12" spans="2:14">
+      <c r="B12" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="36">
+        <v>550</v>
+      </c>
+      <c r="F12" s="47">
+        <f>SUBTOTAL(2,Motorola_Droid_2.1[])/6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G12" s="23">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Sprite])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Sprite])))</f>
+        <v>10.067555</v>
+      </c>
+      <c r="H12" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Animation])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Animation])))</f>
+        <v>9.7792589999999997</v>
+      </c>
+      <c r="I12" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[ShapeModifier])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[ShapeModifier])))</f>
+        <v>17.582723999999999</v>
+      </c>
+      <c r="J12" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[TickerText])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[TickerText])))</f>
+        <v>6.6133508499999998</v>
+      </c>
+      <c r="K12" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[ParticleSystem])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[ParticleSystem])))</f>
+        <v>15.275971999999999</v>
+      </c>
+      <c r="L12" s="30">
+        <f>IF(ISERROR(SUBTOTAL(1,Motorola_Droid_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,Motorola_Droid_2.1[Box2D-Physics])))</f>
+        <v>15.0093785</v>
+      </c>
+      <c r="M12" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>12.388039891666665</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="40">
+      <c r="D13" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="36">
         <v>1000</v>
       </c>
-      <c r="F14" s="47">
-        <f>SUBTOTAL(2,Sony_Ericsson_x10i_1.6[])</f>
-        <v>4</v>
-      </c>
-      <c r="G14" s="24">
+      <c r="F13" s="47">
+        <f>SUBTOTAL(2,Sony_Ericsson_x10i_1.6[])/6</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G13" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Sprite])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Sprite])))</f>
         <v>13.299028</v>
       </c>
-      <c r="H14" s="25">
+      <c r="H13" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Animation])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Animation])))</f>
         <v>8.7267685000000004</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I13" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[ShapeModifier])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[ShapeModifier])))</f>
         <v>12.229005000000001</v>
       </c>
-      <c r="J14" s="25" t="str">
+      <c r="J13" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[TickerText])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[TickerText])))</f>
         <v>?</v>
       </c>
-      <c r="K14" s="25">
+      <c r="K13" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[ParticleSystem])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[ParticleSystem])))</f>
         <v>15.026707999999999</v>
       </c>
-      <c r="L14" s="34" t="str">
+      <c r="L13" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Box2D-Physics])),"?",(SUBTOTAL(1,Sony_Ericsson_x10i_1.6[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M14" s="32">
+      <c r="M13" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>12.320377375</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="40">
+    <row r="14" spans="2:14">
+      <c r="B14" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="36">
         <v>1000</v>
       </c>
-      <c r="F15" s="47">
-        <f>SUBTOTAL(2,HTC_Evo_4G_Supersonic_2.1[])</f>
-        <v>3</v>
-      </c>
-      <c r="G15" s="24" t="str">
+      <c r="F14" s="47">
+        <f>SUBTOTAL(2,HTC_Evo_4G_Supersonic_2.1[])/6</f>
+        <v>0.5</v>
+      </c>
+      <c r="G14" s="23" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Sprite])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Sprite])))</f>
         <v>?</v>
       </c>
-      <c r="H15" s="25">
+      <c r="H14" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Animation])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Animation])))</f>
         <v>11.019192</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I14" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[ShapeModifier])))</f>
         <v>14.979018</v>
       </c>
-      <c r="J15" s="25">
+      <c r="J14" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[TickerText])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[TickerText])))</f>
         <v>10.795321</v>
       </c>
-      <c r="K15" s="25" t="str">
+      <c r="K14" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[ParticleSystem])))</f>
         <v>?</v>
       </c>
-      <c r="L15" s="34" t="str">
+      <c r="L14" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Evo_4G_Supersonic_2.1[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M15" s="32">
+      <c r="M14" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>12.264510333333334</v>
       </c>
     </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="36">
+        <v>528</v>
+      </c>
+      <c r="F15" s="47">
+        <f>SUBTOTAL(2,HTC_Hero_Hiapk_2.18[])/6</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G15" s="23" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Sprite])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Sprite])))</f>
+        <v>?</v>
+      </c>
+      <c r="H15" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Animation])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Animation])))</f>
+        <v>?</v>
+      </c>
+      <c r="I15" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ShapeModifier])))</f>
+        <v>?</v>
+      </c>
+      <c r="J15" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[TickerText])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[TickerText])))</f>
+        <v>?</v>
+      </c>
+      <c r="K15" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ParticleSystem])))</f>
+        <v>6.5550036</v>
+      </c>
+      <c r="L15" s="30">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Box2D-Physics])))</f>
+        <v>5.4402046000000004</v>
+      </c>
+      <c r="M15" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>5.9976041000000002</v>
+      </c>
+    </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="40">
+      <c r="D16" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="36">
         <v>528</v>
       </c>
       <c r="F16" s="47">
-        <f>SUBTOTAL(2,HTC_myTouch3G_1.6[])</f>
+        <f>SUBTOTAL(2,HTC_Hero_Hiapk_2.18[])/6</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G16" s="23">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Sprite])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Sprite])))</f>
+        <v>5.0411853999999998</v>
+      </c>
+      <c r="H16" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Animation])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Animation])))</f>
+        <v>5.1484027000000001</v>
+      </c>
+      <c r="I16" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ShapeModifier])))</f>
+        <v>6.4483629999999996</v>
+      </c>
+      <c r="J16" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[TickerText])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[TickerText])))</f>
+        <v>6.1750499999999997</v>
+      </c>
+      <c r="K16" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ParticleSystem])))</f>
+        <v>?</v>
+      </c>
+      <c r="L16" s="30" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Box2D-Physics])))</f>
+        <v>?</v>
+      </c>
+      <c r="M16" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>5.7032502749999994</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
+      <c r="B17" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="36">
+        <v>528</v>
+      </c>
+      <c r="F17" s="48">
+        <f>SUBTOTAL(2,HTC_Dream_Cyanogen_2.1[])/6</f>
         <v>1</v>
       </c>
-      <c r="G16" s="24" t="str">
+      <c r="G17" s="23">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Sprite])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Sprite])))</f>
+        <v>5.0072136</v>
+      </c>
+      <c r="H17" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Animation])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Animation])))</f>
+        <v>4.5709169999999997</v>
+      </c>
+      <c r="I17" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[ShapeModifier])))</f>
+        <v>6.9393643999999997</v>
+      </c>
+      <c r="J17" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[TickerText])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[TickerText])))</f>
+        <v>5.4820840000000004</v>
+      </c>
+      <c r="K17" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[ParticleSystem])))</f>
+        <v>6.1154102999999997</v>
+      </c>
+      <c r="L17" s="30">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Dream_Cyanogen_2.1[Box2D-Physics])))</f>
+        <v>5.4332867</v>
+      </c>
+      <c r="M17" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>5.5913793333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
+      <c r="B18" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="36">
+        <v>800</v>
+      </c>
+      <c r="F18" s="47">
+        <f>SUBTOTAL(2,Samsung_Galaxy_Spica_2.1[])/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G18" s="23" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Sprite])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Sprite])))</f>
+        <v>?</v>
+      </c>
+      <c r="H18" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Animation])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Animation])))</f>
+        <v>?</v>
+      </c>
+      <c r="I18" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ShapeModifier])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ShapeModifier])))</f>
+        <v>?</v>
+      </c>
+      <c r="J18" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[TickerText])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[TickerText])))</f>
+        <v>?</v>
+      </c>
+      <c r="K18" s="24" t="str">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ParticleSystem])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ParticleSystem])))</f>
+        <v>?</v>
+      </c>
+      <c r="L18" s="30">
+        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Box2D-Physics])))</f>
+        <v>5.2552580000000004</v>
+      </c>
+      <c r="M18" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>5.2552580000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
+      <c r="B19" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="36">
+        <v>528</v>
+      </c>
+      <c r="F19" s="49">
+        <f>SUBTOTAL(2,HTC_Dream_1.6[])/6</f>
+        <v>2</v>
+      </c>
+      <c r="G19" s="23">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Sprite])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Sprite])))</f>
+        <v>3.9721511</v>
+      </c>
+      <c r="H19" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Animation])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Animation])))</f>
+        <v>4.0216501999999998</v>
+      </c>
+      <c r="I19" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Dream_1.6[ShapeModifier])))</f>
+        <v>5.2090484999999997</v>
+      </c>
+      <c r="J19" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[TickerText])),"?",(SUBTOTAL(1,HTC_Dream_1.6[TickerText])))</f>
+        <v>6.6800147000000001</v>
+      </c>
+      <c r="K19" s="24">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Dream_1.6[ParticleSystem])))</f>
+        <v>5.5421003999999998</v>
+      </c>
+      <c r="L19" s="30">
+        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Box2D-Physics])))</f>
+        <v>4.440436</v>
+      </c>
+      <c r="M19" s="52">
+        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
+        <v>4.9775668166666662</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
+      <c r="B20" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="36">
+        <v>528</v>
+      </c>
+      <c r="F20" s="47">
+        <f>SUBTOTAL(2,HTC_myTouch3G_1.6[])/6</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G20" s="23">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[Sprite])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[Sprite])))</f>
-        <v>?</v>
-      </c>
-      <c r="H16" s="25" t="str">
+        <v>4.1197623999999999</v>
+      </c>
+      <c r="H20" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[Animation])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[Animation])))</f>
-        <v>?</v>
-      </c>
-      <c r="I16" s="25" t="str">
+        <v>1.87686</v>
+      </c>
+      <c r="I20" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[ShapeModifier])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[ShapeModifier])))</f>
-        <v>?</v>
-      </c>
-      <c r="J16" s="25">
+        <v>5.5699643999999999</v>
+      </c>
+      <c r="J20" s="24">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[TickerText])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[TickerText])))</f>
-        <v>7.2027340000000004</v>
-      </c>
-      <c r="K16" s="25" t="str">
+        <v>4.7583508500000002</v>
+      </c>
+      <c r="K20" s="24" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[ParticleSystem])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[ParticleSystem])))</f>
         <v>?</v>
       </c>
-      <c r="L16" s="34" t="str">
+      <c r="L20" s="30" t="str">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_myTouch3G_1.6[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_myTouch3G_1.6[Box2D-Physics])))</f>
         <v>?</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M20" s="52">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>7.2027340000000004</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
-      <c r="B17" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="23" t="s">
+        <v>4.0812344124999997</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="15.75" thickBot="1">
+      <c r="B21" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="40">
+      <c r="D21" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="38">
         <v>528</v>
       </c>
-      <c r="F17" s="47">
-        <f>SUBTOTAL(2,HTC_Hero_Hiapk_2.18[])</f>
-        <v>2</v>
-      </c>
-      <c r="G17" s="24" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Sprite])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Sprite])))</f>
-        <v>?</v>
-      </c>
-      <c r="H17" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Animation])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Animation])))</f>
-        <v>?</v>
-      </c>
-      <c r="I17" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ShapeModifier])))</f>
-        <v>?</v>
-      </c>
-      <c r="J17" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[TickerText])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[TickerText])))</f>
-        <v>?</v>
-      </c>
-      <c r="K17" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[ParticleSystem])))</f>
-        <v>6.5550036</v>
-      </c>
-      <c r="L17" s="34">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Hero_Hiapk_2.18[Box2D-Physics])))</f>
-        <v>5.4402046000000004</v>
-      </c>
-      <c r="M17" s="32">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>5.9976041000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
-      <c r="B18" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="40">
-        <v>528</v>
-      </c>
-      <c r="F18" s="46">
-        <f>SUBTOTAL(2,HTC_Hero_Hiapk_2.18[])</f>
-        <v>2</v>
-      </c>
-      <c r="G18" s="24">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Sprite])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Sprite])))</f>
-        <v>5.0411853999999998</v>
-      </c>
-      <c r="H18" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Animation])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Animation])))</f>
-        <v>5.1484027000000001</v>
-      </c>
-      <c r="I18" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ShapeModifier])))</f>
-        <v>6.4483629999999996</v>
-      </c>
-      <c r="J18" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[TickerText])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[TickerText])))</f>
-        <v>6.1750499999999997</v>
-      </c>
-      <c r="K18" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[ParticleSystem])))</f>
-        <v>?</v>
-      </c>
-      <c r="L18" s="34" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Hero_VanillaEclair_4.0[Box2D-Physics])))</f>
-        <v>?</v>
-      </c>
-      <c r="M18" s="32">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>5.7032502749999994</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
-      <c r="B19" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="40">
-        <v>800</v>
-      </c>
-      <c r="F19" s="47">
-        <f>SUBTOTAL(2,Samsung_Galaxy_Spica_2.1[])</f>
-        <v>1</v>
-      </c>
-      <c r="G19" s="24" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Sprite])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Sprite])))</f>
-        <v>?</v>
-      </c>
-      <c r="H19" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Animation])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Animation])))</f>
-        <v>?</v>
-      </c>
-      <c r="I19" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ShapeModifier])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ShapeModifier])))</f>
-        <v>?</v>
-      </c>
-      <c r="J19" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[TickerText])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[TickerText])))</f>
-        <v>?</v>
-      </c>
-      <c r="K19" s="25" t="str">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ParticleSystem])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[ParticleSystem])))</f>
-        <v>?</v>
-      </c>
-      <c r="L19" s="34">
-        <f>IF(ISERROR(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Box2D-Physics])),"?",(SUBTOTAL(1,Samsung_Galaxy_Spica_2.1[Box2D-Physics])))</f>
-        <v>5.2552580000000004</v>
-      </c>
-      <c r="M19" s="32">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>5.2552580000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
-      <c r="B20" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="40">
-        <v>528</v>
-      </c>
-      <c r="F20" s="47">
-        <f>SUBTOTAL(2,HTC_Dream_1.6[])</f>
-        <v>12</v>
-      </c>
-      <c r="G20" s="24">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Sprite])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Sprite])))</f>
-        <v>3.9721511</v>
-      </c>
-      <c r="H20" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Animation])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Animation])))</f>
-        <v>4.0216501999999998</v>
-      </c>
-      <c r="I20" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Dream_1.6[ShapeModifier])))</f>
-        <v>5.2090484999999997</v>
-      </c>
-      <c r="J20" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[TickerText])),"?",(SUBTOTAL(1,HTC_Dream_1.6[TickerText])))</f>
-        <v>6.6800147000000001</v>
-      </c>
-      <c r="K20" s="25">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Dream_1.6[ParticleSystem])))</f>
-        <v>5.5421003999999998</v>
-      </c>
-      <c r="L20" s="34">
-        <f>IF(ISERROR(SUBTOTAL(1,HTC_Dream_1.6[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Dream_1.6[Box2D-Physics])))</f>
-        <v>4.440436</v>
-      </c>
-      <c r="M20" s="32">
-        <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
-        <v>4.9775668166666662</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" ht="15.75" thickBot="1">
-      <c r="B21" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="42">
-        <v>528</v>
-      </c>
-      <c r="F21" s="48">
-        <f>SUBTOTAL(2,HTC_Tattoo_1.6[])</f>
-        <v>10</v>
-      </c>
-      <c r="G21" s="28">
+      <c r="F21" s="50">
+        <f>SUBTOTAL(2,HTC_Tattoo_1.6[])/6</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="G21" s="27">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[Sprite])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[Sprite])))</f>
         <v>3.9166908500000002</v>
       </c>
-      <c r="H21" s="29">
+      <c r="H21" s="28">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[Animation])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[Animation])))</f>
         <v>2.4739784</v>
       </c>
-      <c r="I21" s="29">
+      <c r="I21" s="28">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[ShapeModifier])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[ShapeModifier])))</f>
         <v>5.5150470499999997</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="28">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[TickerText])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[TickerText])))</f>
         <v>1.57046295</v>
       </c>
-      <c r="K21" s="29">
+      <c r="K21" s="28">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[ParticleSystem])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[ParticleSystem])))</f>
         <v>3.4163103000000001</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="31">
         <f>IF(ISERROR(SUBTOTAL(1,HTC_Tattoo_1.6[Box2D-Physics])),"?",(SUBTOTAL(1,HTC_Tattoo_1.6[Box2D-Physics])))</f>
         <v>4.9549089999999998</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="53">
         <f>IF(ISERROR(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])),"?",(AVERAGE(Benchmark[[#This Row],[Sprite]:[Box2D-Physics]])))</f>
         <v>3.6412330916666669</v>
       </c>
@@ -7559,19 +7562,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M5:M21">
-    <cfRule type="colorScale" priority="60">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G5:L21">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7583,7 +7574,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H21">
-    <cfRule type="colorScale" priority="65">
+    <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7595,7 +7586,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I21">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7607,7 +7598,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5:J21">
-    <cfRule type="colorScale" priority="69">
+    <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7619,7 +7610,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:K21">
-    <cfRule type="colorScale" priority="71">
+    <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7631,7 +7622,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5:L21">
-    <cfRule type="colorScale" priority="73">
+    <cfRule type="colorScale" priority="94">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -7643,7 +7634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F21">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="96">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -7654,7 +7645,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E21">
-    <cfRule type="iconSet" priority="1">
+    <cfRule type="iconSet" priority="98">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -7662,6 +7653,18 @@
         <cfvo type="percent" val="60"/>
         <cfvo type="percent" val="80"/>
       </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:G21 H19:L19">
+    <cfRule type="colorScale" priority="100">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7677,10 +7680,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7691,18 +7694,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5">
       <c r="A1" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="23.25">
-      <c r="A2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="15"/>
+      <c r="A2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="62.25">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -7724,227 +7727,257 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.0411853999999998</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.1484027000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.4483629999999996</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6.1750499999999997</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="23.25">
-      <c r="A6" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="A6" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5.0411853999999998</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5.1484027000000001</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.4483629999999996</v>
-      </c>
-      <c r="E7" s="1">
-        <v>6.1750499999999997</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1">
+        <v>6.5550036</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5.4402046000000004</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="23.25">
-      <c r="A9" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="15"/>
+      <c r="A9" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3.9416714000000002</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.4487576</v>
+      </c>
+      <c r="D10" s="1">
+        <v>6.0736264999999996</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.5668987000000001</v>
+      </c>
       <c r="F10" s="1">
-        <v>6.5550036</v>
+        <v>3.4163103000000001</v>
       </c>
       <c r="G10" s="1">
-        <v>5.4402046000000004</v>
+        <v>4.9549089999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="23.25">
-      <c r="A12" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="15"/>
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>1.5740272</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3.8917103000000002</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.4991992000000001</v>
+      </c>
+      <c r="D12" s="1">
+        <v>4.9564675999999999</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1">
-        <v>3.9416714000000002</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.4487576</v>
-      </c>
-      <c r="D13" s="1">
-        <v>6.0736264999999996</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.5668987000000001</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3.4163103000000001</v>
-      </c>
-      <c r="G13" s="1">
-        <v>4.9549089999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1">
-        <v>1.5740272</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" ht="23.25">
+      <c r="A14" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1">
-        <v>3.8917103000000002</v>
+        <v>4.2367743999999998</v>
       </c>
       <c r="C15" s="1">
-        <v>2.4991992000000001</v>
+        <v>4.2539400000000001</v>
       </c>
       <c r="D15" s="1">
-        <v>4.9564675999999999</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+        <v>5.4064819999999996</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.710941</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5.5421003999999998</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4.440436</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="23.25">
-      <c r="A17" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.4784402999999999</v>
+      </c>
+      <c r="C16" s="1">
+        <v>3.5970689999999998</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>7.6490884000000001</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
-        <v>4.2367743999999998</v>
+        <v>4.2012385999999999</v>
       </c>
       <c r="C18" s="1">
-        <v>4.2539400000000001</v>
+        <v>4.2139416000000001</v>
       </c>
       <c r="D18" s="1">
-        <v>5.4064819999999996</v>
-      </c>
-      <c r="E18" s="1">
-        <v>5.710941</v>
-      </c>
-      <c r="F18" s="1">
-        <v>5.5421003999999998</v>
-      </c>
-      <c r="G18" s="1">
-        <v>4.440436</v>
-      </c>
+        <v>5.0116149999999999</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="1">
-        <v>3.4784402999999999</v>
-      </c>
-      <c r="C19" s="1">
-        <v>3.5970689999999998</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1">
-        <v>7.6490884000000001</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+    <row r="20" spans="1:7" ht="23.25">
+      <c r="A20" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
-        <v>4.2012385999999999</v>
+        <v>5.0072136</v>
       </c>
       <c r="C21" s="1">
-        <v>4.2139416000000001</v>
+        <v>4.5709169999999997</v>
       </c>
       <c r="D21" s="1">
-        <v>5.0116149999999999</v>
-      </c>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+        <v>6.9393643999999997</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5.4820840000000004</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6.1154102999999997</v>
+      </c>
+      <c r="G21" s="1">
+        <v>5.4332867</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="12"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="23.25">
-      <c r="A23" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="15"/>
+      <c r="A23" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="1">
         <v>16.069790000000001</v>
@@ -7963,7 +7996,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
@@ -7980,7 +8013,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -7993,7 +8026,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="1">
         <v>12.8821125</v>
@@ -8012,14 +8045,14 @@
       <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="23.25">
-      <c r="A29" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="15"/>
+      <c r="A29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="14"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1">
         <v>17.351126000000001</v>
@@ -8042,44 +8075,44 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1">
-        <v>11.797587</v>
+        <v>15.297293</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1">
-        <v>24.684418000000001</v>
-      </c>
-      <c r="G31" s="1">
-        <v>22.861104999999998</v>
-      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B32" s="1">
+        <v>11.797587</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1">
-        <v>19.625256</v>
-      </c>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1">
+        <v>24.684418000000001</v>
+      </c>
+      <c r="G32" s="1">
+        <v>22.861104999999998</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1">
-        <v>19.663094999999998</v>
-      </c>
-      <c r="E33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1">
+        <v>19.625256</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
@@ -8087,188 +8120,220 @@
       <c r="A34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="1">
-        <v>15.245471999999999</v>
-      </c>
-      <c r="C34" s="1">
-        <v>16.31813</v>
-      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <v>18.253098000000001</v>
+        <v>19.663094999999998</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="3"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="A35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="1">
+        <v>15.245471999999999</v>
+      </c>
+      <c r="C35" s="1">
+        <v>16.31813</v>
+      </c>
+      <c r="D35" s="1">
+        <v>18.253098000000001</v>
+      </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="23.25">
-      <c r="A36" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" s="1">
+    <row r="36" spans="1:7">
+      <c r="A36" s="3"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" ht="23.25">
+      <c r="A37" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="1">
         <v>17.269221999999999</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C38" s="1">
         <v>15.531084999999999</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D38" s="1">
         <v>18.836193000000002</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E38" s="1">
         <v>17.784476999999999</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F38" s="1">
         <v>21.471651000000001</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G38" s="1">
         <v>20.804794000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="3"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="1:7" ht="23.25">
-      <c r="A39" s="18" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="3"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" ht="23.25">
+      <c r="A40" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16">
+        <v>11.735962000000001</v>
+      </c>
+      <c r="D41" s="16">
+        <v>15.083520999999999</v>
+      </c>
+      <c r="E41" s="15"/>
+      <c r="F41" s="16">
+        <v>15.923451999999999</v>
+      </c>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:7" ht="23.25">
+      <c r="A43" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16">
+        <v>9.7283609999999996</v>
+      </c>
+      <c r="E44" s="16">
+        <v>21.894788999999999</v>
+      </c>
+      <c r="F44" s="15">
+        <v>10.11773</v>
+      </c>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="46" spans="1:7" ht="23.25">
+      <c r="A46" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16">
+        <v>7.2027340000000004</v>
+      </c>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="62">
+        <v>4.1197623999999999</v>
+      </c>
+      <c r="C48" s="61">
+        <v>1.87686</v>
+      </c>
+      <c r="D48" s="61">
+        <v>5.5699643999999999</v>
+      </c>
+      <c r="E48" s="61">
+        <v>2.3139677000000001</v>
+      </c>
+      <c r="F48" s="60"/>
+      <c r="G48" s="60"/>
+    </row>
+    <row r="50" spans="1:7" ht="23.25">
+      <c r="A50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="15">
+        <v>13.379421000000001</v>
+      </c>
+      <c r="C51" s="16">
+        <v>11.917116999999999</v>
+      </c>
+      <c r="D51" s="16">
+        <v>15.435746999999999</v>
+      </c>
+      <c r="E51" s="16">
+        <v>15.865864999999999</v>
+      </c>
+      <c r="F51" s="15">
+        <v>15.810184</v>
+      </c>
+      <c r="G51" s="15"/>
+    </row>
+    <row r="53" spans="1:7" ht="23.25">
+      <c r="A53" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="15"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="13" t="s">
+      <c r="C53" s="14"/>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="17">
-        <v>11.735962000000001</v>
-      </c>
-      <c r="D40" s="17">
-        <v>15.083520999999999</v>
-      </c>
-      <c r="E40" s="16"/>
-      <c r="F40" s="17">
-        <v>15.923451999999999</v>
-      </c>
-      <c r="G40" s="16"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="4"/>
-    </row>
-    <row r="42" spans="1:7" ht="23.25">
-      <c r="A42" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="15"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="17">
-        <v>9.7283609999999996</v>
-      </c>
-      <c r="E43" s="17">
-        <v>21.894788999999999</v>
-      </c>
-      <c r="F43" s="16">
-        <v>10.11773</v>
-      </c>
-      <c r="G43" s="16"/>
-    </row>
-    <row r="45" spans="1:7" ht="23.25">
-      <c r="A45" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C45" s="15"/>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17">
-        <v>7.2027340000000004</v>
-      </c>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-    </row>
-    <row r="48" spans="1:7" ht="23.25">
-      <c r="A48" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="15"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="16">
-        <v>13.379421000000001</v>
-      </c>
-      <c r="C49" s="17">
-        <v>11.917116999999999</v>
-      </c>
-      <c r="D49" s="17">
-        <v>15.435746999999999</v>
-      </c>
-      <c r="E49" s="17">
-        <v>15.865864999999999</v>
-      </c>
-      <c r="F49" s="16">
-        <v>15.810184</v>
-      </c>
-      <c r="G49" s="16"/>
-    </row>
-    <row r="51" spans="1:7" ht="23.25">
-      <c r="A51" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="15"/>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="17">
+      <c r="B54" s="15"/>
+      <c r="C54" s="16">
         <v>11.019192</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D54" s="16">
         <v>14.979018</v>
       </c>
-      <c r="E52" s="17">
+      <c r="E54" s="16">
         <v>10.795321</v>
       </c>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <tableParts count="13">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -8281,6 +8346,7 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
@@ -8304,18 +8370,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5">
       <c r="A1" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="23.25">
-      <c r="A2" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="15"/>
+      <c r="A2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="62.25">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -8338,7 +8404,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1">
         <v>13.299028</v>
@@ -8368,10 +8434,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8381,18 +8447,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="33.75">
       <c r="A1" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="23.25">
-      <c r="A2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="15"/>
+      <c r="A2" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="62.25">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -8415,7 +8481,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -8430,57 +8496,80 @@
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="1">
+        <v>10.067555</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.7792589999999997</v>
+      </c>
       <c r="D5" s="1">
-        <v>20.46621</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>14.699237999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>6.1801399999999997</v>
+      </c>
       <c r="F5" s="1">
-        <v>15.621314</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>14.930630000000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>14.493608</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1">
-        <v>7.0465616999999998</v>
-      </c>
-      <c r="F6" s="1"/>
+      <c r="D6" s="1">
+        <v>20.46621</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1">
+        <v>15.621314</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" hidden="1">
+    <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1">
-        <v>10.263685000000001</v>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>7.0465616999999998</v>
+      </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" hidden="1">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1"/>
-      <c r="C8" s="1">
-        <v>2.8178247999999999</v>
-      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1">
-        <v>12.49249</v>
+        <v>10.263685000000001</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" hidden="1">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>2.8178247999999999</v>
+      </c>
+      <c r="D9" s="1">
+        <v>12.49249</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8509,18 +8598,18 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.5">
       <c r="A1" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="26.25">
-      <c r="A2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="15"/>
+      <c r="A2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:7" ht="62.25">
       <c r="A3" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>3</v>
@@ -8543,7 +8632,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>25.367393</v>
@@ -8565,14 +8654,14 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="26.25">
-      <c r="A6" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="15"/>
+      <c r="A6" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <v>5.2552580000000004</v>

</xml_diff>

<commit_message>
Added new SQL-DB backed Benchmarks.xlsx .
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="2" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -19,13 +19,13 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Abfrage von AndEngine Benchmarks" type="1" refreshedVersion="3">
-    <dbPr connection="DRIVER={MySQL ODBC 5.1 Driver};UID=d00e3e7d;SERVER={alekto-programming.com};DATABASE=d00e3e7d;PORT=3306;" command="SELECT t_benchmarks_0.id, t_benchmarks_0.timestamp, t_benchmarks_0.benchmark_id, t_benchmarks_0.benchmark_versionname, t_benchmarks_0.benchmark_versioncode, t_benchmarks_0.benchmark_fps, t_benchmarks_0.device_model, t_benchmarks_0.device_android_version, t_benchmarks_0.device_sdk_version, t_benchmarks_0.device_manufacturer, t_benchmarks_0.device_build_id, t_benchmarks_0.device_build, t_benchmarks_0.device_device, t_benchmarks_0.device_product, t_benchmarks_0.device_cpuabi, t_benchmarks_0.device_board, t_benchmarks_0.device_fingerprint, t_benchmarks_0.benchmark_extension_vbo, t_benchmarks_0.benchmark_extension_drawtexture, t_benchmarks_0.device_imei_x000d__x000a_FROM d00e3e7d.t_benchmarks t_benchmarks_0"/>
+    <dbPr connection="Driver=MySQL ODBC 5.1 Driver;SERVER={alekto-programming.com};UID=d00e3e7d;DATABASE=d00e3e7d;PORT=3306_x0000_" command="SELECT t_benchmarks_0.id, t_benchmarks_0.timestamp, t_benchmarks_0.benchmark_id, t_benchmarks_0.benchmark_versionname, t_benchmarks_0.benchmark_versioncode, t_benchmarks_0.benchmark_fps, t_benchmarks_0.device_model, t_benchmarks_0.device_android_version, t_benchmarks_0.device_sdk_version, t_benchmarks_0.device_manufacturer, t_benchmarks_0.device_build_id, t_benchmarks_0.device_build, t_benchmarks_0.device_device, t_benchmarks_0.device_product, t_benchmarks_0.device_cpuabi, t_benchmarks_0.device_board, t_benchmarks_0.device_fingerprint, t_benchmarks_0.benchmark_extension_vbo, t_benchmarks_0.benchmark_extension_drawtexture, t_benchmarks_0.device_imei_x000d__x000a_FROM d00e3e7d.t_benchmarks t_benchmarks_0"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>TickerText</t>
   </si>
@@ -76,6 +76,39 @@
   </si>
   <si>
     <t>Bench</t>
+  </si>
+  <si>
+    <t>GT-I9000</t>
+  </si>
+  <si>
+    <t>Liquid</t>
+  </si>
+  <si>
+    <t>HTC Desire</t>
+  </si>
+  <si>
+    <t>ADR6300</t>
+  </si>
+  <si>
+    <t>XT720</t>
+  </si>
+  <si>
+    <t>Droid</t>
+  </si>
+  <si>
+    <t>A853</t>
+  </si>
+  <si>
+    <t>E10i</t>
+  </si>
+  <si>
+    <t>HTC Magic</t>
+  </si>
+  <si>
+    <t>Docomo HT-03A</t>
+  </si>
+  <si>
+    <t>X10i</t>
   </si>
 </sst>
 </file>
@@ -363,340 +396,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="109">
-    <dxf>
-      <alignment textRotation="70" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="70" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="75">
     <dxf>
       <alignment textRotation="70" readingOrder="0"/>
     </dxf>
@@ -1443,13 +1143,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium16 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="108"/>
-      <tableStyleElement type="headerRow" dxfId="107"/>
-      <tableStyleElement type="totalRow" dxfId="106"/>
-      <tableStyleElement type="firstColumn" dxfId="105"/>
-      <tableStyleElement type="lastColumn" dxfId="104"/>
-      <tableStyleElement type="firstRowStripe" dxfId="103"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="102"/>
+      <tableStyleElement type="wholeTable" dxfId="74"/>
+      <tableStyleElement type="headerRow" dxfId="73"/>
+      <tableStyleElement type="totalRow" dxfId="72"/>
+      <tableStyleElement type="firstColumn" dxfId="71"/>
+      <tableStyleElement type="lastColumn" dxfId="70"/>
+      <tableStyleElement type="firstRowStripe" dxfId="69"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="68"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -1594,16 +1294,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1611,18 +1344,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$C$8:$C$11</c:f>
+              <c:f>Benchmarks!$C$8:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>17.226800000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
+                  <c:v>22.449300000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.426416666666668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.268999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.206900000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0224499999999992</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.6301400000000008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.7490299999999994</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>4.0504699999999998</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.7688299999999999</c:v>
+                <c:pt idx="13">
+                  <c:v>3.86246</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1644,16 +1395,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1661,17 +1445,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$D$8:$D$11</c:f>
+              <c:f>Benchmarks!$D$8:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>16.032900000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.3552099999999996</c:v>
+                  <c:v>21.101299999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>15.580750000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.283100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.386099999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.730399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.6300400000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.1149</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.639699999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.3078699999999994</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>2.5402200000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1694,16 +1499,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1711,17 +1549,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$E$8:$E$11</c:f>
+              <c:f>Benchmarks!$E$8:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>19.675999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.65693</c:v>
+                  <c:v>30.263500000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>19.538999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.2423</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.834299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.2303</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.94285</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.442399999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.36</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5901449999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>5.7587000000000002</c:v>
                 </c:pt>
               </c:numCache>
@@ -1744,16 +1603,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1761,17 +1653,38 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$F$8:$F$11</c:f>
+              <c:f>Benchmarks!$F$8:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>19.587599999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.5746200000000004</c:v>
+                  <c:v>23.0059</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>19.592833333333331</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.5276</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.454499999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.357900000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.2748499999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2275900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.8972300000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.9780700000000007</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1.6008500000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1794,16 +1707,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1811,17 +1757,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$G$8:$G$11</c:f>
+              <c:f>Benchmarks!$G$8:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>25.982500000000002</c:v>
+                  <c:v>25.753799999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>24.884699999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.333350000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.6311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.866849999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.2043</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.9395799999999994</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.4039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.9245</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>6.1369600000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="13">
                   <c:v>3.3304100000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -1844,16 +1814,49 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Benchmarks!$B$8:$B$11</c:f>
+              <c:f>Benchmarks!$B$8:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>GT-I9000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Liquid</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Nexus One</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
+                  <c:v>HTC Desire</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>ADR6300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>X10i</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>XT720</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>E10i</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Droid</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>A853</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>HTC Magic</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>T-Mobile G1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
+                  <c:v>Docomo HT-03A</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>HTC Tattoo</c:v>
                 </c:pt>
               </c:strCache>
@@ -1861,41 +1864,65 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Benchmarks!$H$8:$H$11</c:f>
+              <c:f>Benchmarks!$H$8:$H$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>23.358899999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4875100000000003</c:v>
+                  <c:v>31.088799999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>23.238939999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.072200000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.0868</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.1531</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.343400000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.3736</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7200300000000004</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.6874649999999995</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2819700000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>5.0047800000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="75620736"/>
-        <c:axId val="75622272"/>
+        <c:axId val="67050112"/>
+        <c:axId val="67068288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75620736"/>
+        <c:axId val="67050112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75622272"/>
+        <c:crossAx val="67068288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75622272"/>
+        <c:axId val="67068288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1903,7 +1930,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75620736"/>
+        <c:crossAx val="67050112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1916,7 +1943,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000018" r="0.70000000000000018" t="0.78740157499999996" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7000000000000004" r="0.7000000000000004" t="0.78740157499999996" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1958,52 +1985,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40361.821456365738" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="18">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40363.862021759262" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="94">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="20">
     <cacheField name="id" numFmtId="0" sqlType="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="29" count="18">
-        <n v="16"/>
-        <n v="12"/>
-        <n v="15"/>
-        <n v="13"/>
-        <n v="14"/>
-        <n v="17"/>
-        <n v="18"/>
-        <n v="19"/>
-        <n v="20"/>
-        <n v="21"/>
-        <n v="22"/>
-        <n v="23"/>
-        <n v="24"/>
-        <n v="25"/>
-        <n v="26"/>
-        <n v="27"/>
-        <n v="28"/>
-        <n v="29"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="105"/>
     </cacheField>
     <cacheField name="timestamp" numFmtId="0" sqlType="11">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-02T17:29:02" count="18">
-        <d v="2010-07-02T17:08:17"/>
-        <d v="2010-07-02T17:05:18"/>
-        <d v="2010-07-02T17:07:44"/>
-        <d v="2010-07-02T17:06:02"/>
-        <d v="2010-07-02T17:07:16"/>
-        <d v="2010-07-02T17:09:44"/>
-        <d v="2010-07-02T17:23:13"/>
-        <d v="2010-07-02T17:23:54"/>
-        <d v="2010-07-02T17:25:41"/>
-        <d v="2010-07-02T17:25:48"/>
-        <d v="2010-07-02T17:26:08"/>
-        <d v="2010-07-02T17:26:47"/>
-        <d v="2010-07-02T17:27:15"/>
-        <d v="2010-07-02T17:27:27"/>
-        <d v="2010-07-02T17:27:40"/>
-        <d v="2010-07-02T17:28:27"/>
-        <d v="2010-07-02T17:28:28"/>
-        <d v="2010-07-02T17:29:02"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-04T19:43:33"/>
     </cacheField>
     <cacheField name="benchmark_id" numFmtId="0" sqlType="4">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5" count="6">
@@ -2019,9 +2008,9 @@
       <sharedItems count="5">
         <s v="1.1.5"/>
         <s v="" u="1"/>
+        <s v="1.1.3" u="1"/>
+        <s v="1.1.4" u="1"/>
         <s v="benchmark_versionname" u="1"/>
-        <s v="1.1.4" u="1"/>
-        <s v="1.1.3" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_versioncode" numFmtId="0" sqlType="4">
@@ -2030,32 +2019,24 @@
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_fps" numFmtId="0" sqlType="7">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.6008500000000001" maxValue="25.982500000000002" count="18">
-        <n v="25.982500000000002"/>
-        <n v="19.675999999999998"/>
-        <n v="19.587599999999998"/>
-        <n v="17.226800000000001"/>
-        <n v="16.032900000000001"/>
-        <n v="23.358899999999998"/>
-        <n v="3.7688299999999999"/>
-        <n v="5.7587000000000002"/>
-        <n v="2.5402200000000001"/>
-        <n v="4.0504699999999998"/>
-        <n v="5.65693"/>
-        <n v="1.6008500000000001"/>
-        <n v="4.3552099999999996"/>
-        <n v="3.3304100000000001"/>
-        <n v="7.5746200000000004"/>
-        <n v="6.1369600000000002"/>
-        <n v="5.0047800000000002"/>
-        <n v="4.4875100000000003"/>
-      </sharedItems>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.6008500000000001" maxValue="31.088799999999999"/>
     </cacheField>
     <cacheField name="device_model" numFmtId="0" sqlType="12">
-      <sharedItems count="7">
+      <sharedItems count="18">
         <s v="Nexus One"/>
         <s v="HTC Tattoo"/>
         <s v="T-Mobile G1"/>
+        <s v="Liquid"/>
+        <s v="GT-I9000"/>
+        <s v="Droid"/>
+        <s v="XT720"/>
+        <s v="HTC Magic"/>
+        <s v="A853"/>
+        <s v="E10i"/>
+        <s v="Docomo HT-03A"/>
+        <s v="HTC Desire"/>
+        <s v="ADR6300"/>
+        <s v="X10i"/>
         <s v="" u="1"/>
         <s v="HTC Wildfire" u="1"/>
         <s v="device_model" u="1"/>
@@ -2066,52 +2047,107 @@
       <sharedItems count="7">
         <s v="2.2"/>
         <s v="1.6"/>
+        <s v="2.1-update1"/>
         <s v="" u="1"/>
-        <s v="2.1-update1" u="1"/>
-        <s v="2.1" u="1"/>
         <s v="device_android_version_2" u="1"/>
         <s v="device_android_version" u="1"/>
+        <s v="2.1" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_sdk_version" numFmtId="0" sqlType="5">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="8" count="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="8" count="3">
         <n v="8"/>
         <n v="4"/>
+        <n v="7"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_manufacturer" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="7">
         <s v="HTC"/>
+        <s v="Acer"/>
+        <s v="samsung"/>
+        <s v="Motorola"/>
+        <s v="Sony Ericsson"/>
         <s v="" u="1"/>
         <s v="device_manufacturer" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_build_id" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="16">
         <s v="FRF91"/>
         <s v="DRC79"/>
         <s v="DMD64"/>
+        <s v="FRF50"/>
+        <s v="ECLAIR"/>
+        <s v="ESE81"/>
+        <s v="STSKT_N_79.11.36R1"/>
+        <s v="ERD79"/>
+        <s v="SHLA_U2_03.05.0"/>
+        <s v="1.0.A.1.36"/>
+        <s v="DRD08"/>
+        <s v="FRF85b"/>
+        <s v="1.0.A.1.38"/>
+        <s v="ERE27"/>
+        <s v="DRC83"/>
+        <s v="R1FB001"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_build" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="17">
         <s v="FRF91"/>
         <s v="DRC79"/>
         <s v="DMD64"/>
+        <s v="FRF50_Liquid-Port"/>
+        <s v="ECLAIR"/>
+        <s v="ESE81"/>
+        <s v="STSKT_N_79.11.36R1"/>
+        <s v="Smoki_0.6.9"/>
+        <s v="SHLA_U2_03.05.0"/>
+        <s v="1.0.A.1.36"/>
+        <s v="FRF91 MRCr21/CM6 Mod By RoDrIgUeZsTyLe"/>
+        <s v="DRD08"/>
+        <s v="DeFroST 1.6c for HTC Desire (FRF85b)"/>
+        <s v="1.0.A.1.38"/>
+        <s v="ERE27"/>
+        <s v="AOSP-1.6_r2-DRD36_v2.6.3"/>
+        <s v="R1FB001"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_device" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="13">
         <s v="passion"/>
         <s v="bahamas"/>
         <s v="dream"/>
+        <s v="a1"/>
+        <s v="GT-I9000"/>
+        <s v="sholes"/>
+        <s v="sholest"/>
+        <s v="sapphire"/>
+        <s v="umts_sholes"/>
+        <s v="SonyEricssonE10i"/>
+        <s v="inc"/>
+        <s v="bravo"/>
+        <s v="SonyEricssonX10i"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_product" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="16">
         <s v="passion"/>
         <s v="htc_tattoo"/>
         <s v="kila"/>
+        <s v="a1_generic1"/>
+        <s v="GT-I9000"/>
+        <s v="voles"/>
+        <s v="sholest_skt"/>
+        <s v="htc_magic"/>
+        <s v="umts_sholes"/>
+        <s v="E10i_1237-2935"/>
+        <s v="zaku"/>
+        <s v="E10i_1238-0549"/>
+        <s v="inc"/>
+        <s v="htc_bravo"/>
+        <s v="E10i_1237-1322"/>
+        <s v="X10_1234-8465"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_cpuabi" numFmtId="0" sqlType="12">
@@ -2121,17 +2157,40 @@
       </sharedItems>
     </cacheField>
     <cacheField name="device_board" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="11">
         <s v="mahimahi"/>
         <s v="bahamas"/>
         <s v="trout"/>
+        <s v="salsa"/>
+        <s v="GT-I9000"/>
+        <s v="sholes"/>
+        <s v="sapphire"/>
+        <s v="delta"/>
+        <s v="bravo"/>
+        <s v="inc"/>
+        <s v="es209ra"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_fingerprint" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="18">
         <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
         <s v="htc_wwe/htc_tattoo/bahamas/bahamas:1.6/DRC79/74178:user/release-keys"/>
         <s v="tmobile/kila/dream/trout:1.6/DMD64/21415:user/ota-rel-keys,release-keys"/>
+        <s v="acer/a1_generic1/a1/salsa:2.2/FRF50/38042:user/release-keys"/>
+        <s v="Samsung/GT-I9000/GT-I9000/GT-I9000:2.1-update1/ECLAIR/DXJF4:user/release-keys"/>
+        <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+        <s v="MOT/sholest_skt/sholest/sholes:2.1-update1/STSKT_N_79.11.36R1/0423:user/release-keys"/>
+        <s v="google/passion/passion/mahimahi:2.1/ERD79/22607:user/release-keys"/>
+        <s v="MOTO_TIMBR/umts_sholes/umts_sholes/sholes:2.1-update1/SHLA_U2_03.05.0/8935007:user/rel-keys"/>
+        <s v="SEMC/E10i_1237-2935/SonyEricssonE10i/delta:1.6/1.0.A.1.36/0:user/release-keys"/>
+        <s v="docomo/zaku/sapphire/sapphire:1.6/DRD08/16431:user/ota-rel-keys,release-keys"/>
+        <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+        <s v="SEMC/E10i_1238-0549/SonyEricssonE10i/delta:1.6/1.0.A.1.38/0:user/release-keys"/>
+        <s v="verizon/inc/inc/inc:2.1-update1/ERE27/161494:user/release-keys"/>
+        <s v="htc_wwe/htc_bravo/bravo/bravo:2.1-update1/ERE27/174215:user/release-keys"/>
+        <s v="SEMC/E10i_1237-1322/SonyEricssonE10i/delta:1.6/1.0.A.1.38/0:user/release-keys"/>
+        <s v="tmobile/kila/dream/trout:1.6/DRC83/14721:user/ota-rel-keys,release-keys"/>
+        <s v="SEMC/X10_1234-8465/SonyEricssonX10i/es209ra:1.6/R1FB001/1270087315:user/rel-keys"/>
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_extension_vbo" numFmtId="0" sqlType="-6">
@@ -2146,10 +2205,31 @@
       </sharedItems>
     </cacheField>
     <cacheField name="device_imei" numFmtId="0" sqlType="12">
-      <sharedItems count="3">
+      <sharedItems count="24">
         <s v="354957032594197"/>
         <s v="358355021486002"/>
         <s v="358279011512835"/>
+        <s v="353509030068160"/>
+        <s v="351751040120373"/>
+        <s v="A0000015FCAD39"/>
+        <s v="354636030642188"/>
+        <s v="354957032587928"/>
+        <s v="354059027532645"/>
+        <s v="356698030279856"/>
+        <s v="012312004112087"/>
+        <s v="354957031553616"/>
+        <s v="358098020840239"/>
+        <s v="357841030201509"/>
+        <s v="012312001091797"/>
+        <s v="A100001351BB96"/>
+        <s v="351680031197837"/>
+        <s v="354957032398417"/>
+        <s v="357841031973593"/>
+        <s v="012312002777386"/>
+        <s v="358279017179100"/>
+        <s v="354957030769916"/>
+        <s v="354957031494423"/>
+        <s v="359419030331143"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -2157,409 +2237,2081 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="18">
-  <r>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="94">
+  <r>
+    <n v="16"/>
+    <d v="2010-07-02T17:08:17"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.982500000000002"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <d v="2010-07-02T17:05:18"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.675999999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="15"/>
+    <d v="2010-07-02T17:07:44"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.587599999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="13"/>
+    <d v="2010-07-02T17:06:02"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.226800000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="14"/>
+    <d v="2010-07-02T17:07:16"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.032900000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="17"/>
+    <d v="2010-07-02T17:09:44"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.358899999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="18"/>
+    <d v="2010-07-02T17:23:13"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.7688299999999999"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="19"/>
+    <d v="2010-07-02T17:23:54"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.7587000000000002"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="20"/>
+    <d v="2010-07-02T17:25:41"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2.5402200000000001"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="21"/>
+    <d v="2010-07-02T17:25:48"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.0504699999999998"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="22"/>
+    <d v="2010-07-02T17:26:08"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.65693"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="23"/>
+    <d v="2010-07-02T17:26:47"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.6008500000000001"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="24"/>
+    <d v="2010-07-02T17:27:15"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.3552099999999996"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="25"/>
+    <d v="2010-07-02T17:27:27"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.3304100000000001"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="26"/>
+    <d v="2010-07-02T17:27:40"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.5746200000000004"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="27"/>
+    <d v="2010-07-02T17:28:27"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.1369600000000002"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="28"/>
+    <d v="2010-07-02T17:28:28"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.0047800000000002"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="29"/>
+    <d v="2010-07-02T17:29:02"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.4875100000000003"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="30"/>
+    <d v="2010-07-03T15:07:40"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.360299999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="31"/>
+    <d v="2010-07-03T15:20:01"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.9560900000000001"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="32"/>
+    <d v="2010-07-03T15:51:59"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="24.884699999999999"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
     <x v="3"/>
     <x v="3"/>
     <x v="3"/>
-    <x v="0"/>
-    <x v="0"/>
     <x v="3"/>
     <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <x v="4"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <x v="5"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="0"/>
-  </r>
-  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="33"/>
+    <d v="2010-07-03T17:07:49"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="22.449300000000001"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="34"/>
+    <d v="2010-07-03T17:08:12"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="30.263500000000001"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="35"/>
+    <d v="2010-07-03T17:08:43"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="21.101299999999998"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="36"/>
+    <d v="2010-07-03T17:09:05"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.0059"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="37"/>
+    <d v="2010-07-03T17:09:45"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.753799999999998"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="38"/>
+    <d v="2010-07-03T17:10:15"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="31.088799999999999"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <n v="39"/>
+    <d v="2010-07-03T18:57:03"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.442399999999999"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="40"/>
+    <d v="2010-07-03T18:57:31"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.1149"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="41"/>
+    <d v="2010-07-03T18:57:52"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.2748499999999998"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="42"/>
+    <d v="2010-07-03T18:58:19"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.4039"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="43"/>
+    <d v="2010-07-03T18:58:48"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="13.343400000000001"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="44"/>
+    <d v="2010-07-03T18:59:08"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9.6301400000000008"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <n v="45"/>
+    <d v="2010-07-03T21:12:29"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.2303"/>
+    <x v="6"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="6"/>
     <x v="6"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <n v="46"/>
+    <d v="2010-07-03T21:40:01"/>
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
-    <x v="6"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+    <n v="14.8939"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="47"/>
+    <d v="2010-07-03T21:40:27"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.467000000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="48"/>
+    <d v="2010-07-03T21:41:31"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.058299999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="49"/>
+    <d v="2010-07-03T21:41:55"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.525300000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="50"/>
+    <d v="2010-07-03T21:42:25"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.680299999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="51"/>
+    <d v="2010-07-03T21:42:57"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.592199999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <n v="52"/>
+    <d v="2010-07-03T23:00:53"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.7200300000000004"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
     <x v="7"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="0"/>
     <x v="7"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="53"/>
+    <d v="2010-07-03T23:01:20"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.8972300000000004"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="7"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <n v="54"/>
+    <d v="2010-07-04T00:13:55"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9.7490299999999994"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
     <x v="8"/>
     <x v="8"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
     <x v="8"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="55"/>
+    <d v="2010-07-04T00:14:20"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.36"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="56"/>
+    <d v="2010-07-04T00:14:41"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.639699999999999"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="57"/>
+    <d v="2010-07-04T00:15:06"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.2275900000000002"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="58"/>
+    <d v="2010-07-04T00:15:41"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="13.9245"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="59"/>
+    <d v="2010-07-04T00:16:13"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12.3736"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="1"/>
+    <x v="5"/>
+    <x v="8"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <n v="60"/>
+    <d v="2010-07-04T00:19:15"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.1531"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
     <x v="9"/>
     <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="61"/>
+    <d v="2010-07-04T00:19:51"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="8.9395799999999994"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="62"/>
+    <d v="2010-07-04T00:20:12"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="20.0702"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="63"/>
+    <d v="2010-07-04T00:20:33"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.6300400000000002"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="64"/>
+    <d v="2010-07-04T00:20:52"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="11.279500000000001"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+  </r>
+  <r>
+    <n v="65"/>
+    <d v="2010-07-04T00:21:17"/>
     <x v="3"/>
     <x v="0"/>
     <x v="0"/>
+    <n v="8.0224499999999992"/>
     <x v="9"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="9"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="10"/>
+  </r>
+  <r>
+    <n v="66"/>
+    <d v="2010-07-04T01:19:48"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="21.995799999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="10"/>
-    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="67"/>
+    <d v="2010-07-04T01:20:21"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.601800000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="0"/>
     <x v="0"/>
     <x v="10"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="11"/>
+  </r>
+  <r>
+    <n v="68"/>
+    <d v="2010-07-04T01:20:41"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.8827"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="11"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
+  </r>
+  <r>
+    <n v="69"/>
+    <d v="2010-07-04T01:20:41"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.2819700000000003"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="10"/>
     <x v="11"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+    <x v="7"/>
+    <x v="10"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="12"/>
+  </r>
+  <r>
+    <n v="70"/>
+    <d v="2010-07-04T01:21:00"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.4452"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="71"/>
+    <d v="2010-07-04T01:21:19"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.665600000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="72"/>
+    <d v="2010-07-04T01:21:48"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.441500000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="73"/>
+    <d v="2010-07-04T01:22:20"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.663399999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+  </r>
+  <r>
+    <n v="74"/>
+    <d v="2010-07-04T03:31:17"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.283100000000001"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
     <x v="12"/>
-    <x v="4"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="75"/>
+    <d v="2010-07-04T03:31:39"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.2423"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
     <x v="12"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="13"/>
+  </r>
+  <r>
+    <n v="76"/>
+    <d v="2010-07-04T03:32:02"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.268999999999998"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="13"/>
-    <x v="0"/>
+  </r>
+  <r>
+    <n v="77"/>
+    <d v="2010-07-04T03:32:22"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.5276"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
     <x v="0"/>
     <x v="0"/>
     <x v="13"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <n v="78"/>
+    <d v="2010-07-04T03:32:49"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.6311"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="79"/>
+    <d v="2010-07-04T03:33:17"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="22.7042"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="13"/>
+  </r>
+  <r>
+    <n v="80"/>
+    <d v="2010-07-04T05:23:48"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.606199999999999"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="12"/>
+    <x v="13"/>
+    <x v="9"/>
+    <x v="11"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="14"/>
+  </r>
+  <r>
+    <n v="81"/>
+    <d v="2010-07-04T05:39:30"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.294600000000001"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
     <x v="14"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="82"/>
+    <d v="2010-07-04T05:39:47"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12.664899999999999"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
     <x v="14"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="15"/>
+  </r>
+  <r>
+    <n v="83"/>
+    <d v="2010-07-04T05:40:10"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="11.8987"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="0"/>
     <x v="15"/>
-    <x v="0"/>
+  </r>
+  <r>
+    <n v="84"/>
+    <d v="2010-07-04T05:40:28"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="18.4435"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
     <x v="0"/>
     <x v="0"/>
     <x v="15"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
-  </r>
-  <r>
+  </r>
+  <r>
+    <n v="85"/>
+    <d v="2010-07-04T05:40:52"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.967400000000001"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="86"/>
+    <d v="2010-07-04T05:41:19"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.6876"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="87"/>
+    <d v="2010-07-04T05:42:08"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="13.748900000000001"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="88"/>
+    <d v="2010-07-04T05:42:24"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.373999999999999"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="89"/>
+    <d v="2010-07-04T05:42:42"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12.8735"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="90"/>
+    <d v="2010-07-04T05:42:59"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="18.465499999999999"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="91"/>
+    <d v="2010-07-04T05:43:23"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.766300000000001"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="92"/>
+    <d v="2010-07-04T05:43:49"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="20.486000000000001"/>
+    <x v="12"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="10"/>
+    <x v="12"/>
+    <x v="0"/>
+    <x v="9"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="15"/>
+  </r>
+  <r>
+    <n v="93"/>
+    <d v="2010-07-04T08:43:05"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.5233599999999998"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
     <x v="16"/>
+  </r>
+  <r>
+    <n v="94"/>
+    <d v="2010-07-04T12:21:02"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.683"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="17"/>
+  </r>
+  <r>
+    <n v="95"/>
+    <d v="2010-07-04T13:10:15"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.440200000000001"/>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="13"/>
+    <x v="14"/>
+    <x v="11"/>
+    <x v="13"/>
+    <x v="0"/>
+    <x v="8"/>
+    <x v="14"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="18"/>
+  </r>
+  <r>
+    <n v="96"/>
+    <d v="2010-07-04T15:57:32"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="18.645600000000002"/>
+    <x v="9"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="12"/>
+    <x v="13"/>
+    <x v="9"/>
+    <x v="14"/>
+    <x v="1"/>
+    <x v="7"/>
+    <x v="15"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="19"/>
+  </r>
+  <r>
+    <n v="97"/>
+    <d v="2010-07-04T17:43:38"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.2605300000000002"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="16"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <n v="98"/>
+    <d v="2010-07-04T17:44:31"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.3815200000000001"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
     <x v="16"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-  </r>
-  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <n v="99"/>
+    <d v="2010-07-04T17:45:10"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.8874199999999997"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="14"/>
+    <x v="15"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="16"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="20"/>
+  </r>
+  <r>
+    <n v="100"/>
+    <d v="2010-07-04T18:08:02"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.584399999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <n v="101"/>
+    <d v="2010-07-04T18:08:23"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.3779"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <n v="102"/>
+    <d v="2010-07-04T18:08:51"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="24.229099999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="21"/>
+  </r>
+  <r>
+    <n v="103"/>
+    <d v="2010-07-04T18:47:10"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.7927"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="22"/>
+  </r>
+  <r>
+    <n v="104"/>
+    <d v="2010-07-04T19:43:10"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="22.2043"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="15"/>
+    <x v="16"/>
+    <x v="12"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="10"/>
     <x v="17"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="23"/>
+  </r>
+  <r>
+    <n v="105"/>
+    <d v="2010-07-04T19:43:33"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.730399999999999"/>
+    <x v="13"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="4"/>
+    <x v="15"/>
+    <x v="16"/>
+    <x v="12"/>
+    <x v="15"/>
+    <x v="1"/>
+    <x v="10"/>
     <x v="17"/>
-    <x v="5"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="17"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="1"/>
-    <x v="0"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="1"/>
-    <x v="2"/>
-    <x v="2"/>
-    <x v="0"/>
-    <x v="0"/>
-    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="23"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
-  <location ref="B6:I11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
+  <location ref="B6:I22" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -2577,8 +4329,8 @@
     <pivotField name="Benchmark Version" axis="axisPage" showAll="0">
       <items count="6">
         <item m="1" x="3"/>
+        <item m="1" x="2"/>
         <item m="1" x="4"/>
-        <item m="1" x="2"/>
         <item m="1" x="1"/>
         <item x="0"/>
         <item t="default"/>
@@ -2587,14 +4339,25 @@
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0" countASubtotal="1"/>
     <pivotField name="Device" axis="axisRow" showAll="0" sortType="descending">
-      <items count="8">
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="3"/>
+      <items count="19">
+        <item m="1" x="15"/>
+        <item m="1" x="17"/>
+        <item m="1" x="16"/>
+        <item m="1" x="14"/>
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
         <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
       <autoSortScope>
@@ -2609,22 +4372,26 @@
     </pivotField>
     <pivotField name="Android Version" axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="8">
+        <item m="1" x="5"/>
+        <item m="1" x="4"/>
+        <item x="2"/>
         <item m="1" x="6"/>
-        <item m="1" x="5"/>
+        <item x="0"/>
         <item m="1" x="3"/>
-        <item m="1" x="4"/>
-        <item x="0"/>
-        <item m="1" x="2"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField name="Manufacturer" axis="axisPage" showAll="0">
-      <items count="4">
-        <item m="1" x="2"/>
+      <items count="8">
+        <item m="1" x="6"/>
         <item x="0"/>
-        <item m="1" x="1"/>
+        <item m="1" x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2642,12 +4409,45 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="15">
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
     <i>
       <x v="4"/>
     </i>
     <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
       <x v="6"/>
+    </i>
+    <i>
+      <x v="14"/>
     </i>
     <i>
       <x v="5"/>
@@ -2691,174 +4491,158 @@
     <dataField name="FPS" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="34">
-    <format dxfId="101">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="98">
+    <format dxfId="64">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="63">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="61">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="60">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="59">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="58">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="91">
+    <format dxfId="57">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="90">
+    <format dxfId="56">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="55">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="54">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="53">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="52">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="51">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="50">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="49">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="48">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="47">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="80">
+    <format dxfId="46">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="78">
+    <format dxfId="44">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="77">
+    <format dxfId="43">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="42">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="41">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="40">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="73">
+    <format dxfId="39">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="38">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="71">
+    <format dxfId="37">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="36">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="35">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="68">
+    <format dxfId="34">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
   </formats>
   <conditionalFormats count="7">
-    <conditionalFormat priority="8">
-      <pivotAreas count="1">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="6" count="3">
-              <x v="4"/>
-              <x v="5"/>
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
     <conditionalFormat priority="7">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -2867,12 +4651,23 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="1"/>
+              <x v="0"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -2886,12 +4681,23 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="2"/>
+              <x v="1"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -2905,12 +4711,23 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="3"/>
+              <x v="2"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -2924,12 +4741,23 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="4"/>
+              <x v="3"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -2943,12 +4771,23 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="5"/>
+              <x v="4"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -2962,12 +4801,50 @@
               <x v="0"/>
             </reference>
             <reference field="2" count="1" selected="0">
-              <x v="0"/>
+              <x v="5"/>
             </reference>
-            <reference field="6" count="3">
+            <reference field="6" count="14">
               <x v="4"/>
               <x v="5"/>
               <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="6" count="14">
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+              <x v="9"/>
+              <x v="10"/>
+              <x v="11"/>
+              <x v="12"/>
+              <x v="13"/>
+              <x v="14"/>
+              <x v="15"/>
+              <x v="16"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -3340,10 +5217,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B2:I17"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3426,125 +5303,350 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="9" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C8" s="10">
-        <v>17.226800000000001</v>
+        <v>22.449300000000001</v>
       </c>
       <c r="D8" s="11">
-        <v>16.032900000000001</v>
+        <v>21.101299999999998</v>
       </c>
       <c r="E8" s="11">
-        <v>19.675999999999998</v>
+        <v>30.263500000000001</v>
       </c>
       <c r="F8" s="11">
-        <v>19.587599999999998</v>
+        <v>23.0059</v>
       </c>
       <c r="G8" s="11">
-        <v>25.982500000000002</v>
+        <v>25.753799999999998</v>
       </c>
       <c r="H8" s="11">
-        <v>23.358899999999998</v>
+        <v>31.088799999999999</v>
       </c>
       <c r="I8" s="12">
-        <v>20.310783333333333</v>
+        <v>25.610433333333333</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15">
+        <v>24.884699999999999</v>
+      </c>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16">
+        <v>24.884699999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="14">
+        <v>16.426416666666668</v>
+      </c>
+      <c r="D10" s="15">
+        <v>15.580750000000002</v>
+      </c>
+      <c r="E10" s="15">
+        <v>19.538999999999998</v>
+      </c>
+      <c r="F10" s="15">
+        <v>19.592833333333331</v>
+      </c>
+      <c r="G10" s="15">
+        <v>25.333350000000003</v>
+      </c>
+      <c r="H10" s="15">
+        <v>23.238939999999999</v>
+      </c>
+      <c r="I10" s="16">
+        <v>19.832204000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="14">
+        <v>16.268999999999998</v>
+      </c>
+      <c r="D11" s="15">
+        <v>16.283100000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <v>19.2423</v>
+      </c>
+      <c r="F11" s="15">
+        <v>19.5276</v>
+      </c>
+      <c r="G11" s="15">
+        <v>25.6311</v>
+      </c>
+      <c r="H11" s="15">
+        <v>19.072200000000002</v>
+      </c>
+      <c r="I11" s="16">
+        <v>19.299642857142857</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14">
+        <v>13.206900000000001</v>
+      </c>
+      <c r="D12" s="15">
+        <v>12.386099999999999</v>
+      </c>
+      <c r="E12" s="15">
+        <v>15.834299999999999</v>
+      </c>
+      <c r="F12" s="15">
+        <v>18.454499999999999</v>
+      </c>
+      <c r="G12" s="15">
+        <v>18.866849999999999</v>
+      </c>
+      <c r="H12" s="15">
+        <v>20.0868</v>
+      </c>
+      <c r="I12" s="16">
+        <v>16.472574999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15">
+        <v>10.730399999999999</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15">
+        <v>22.2043</v>
+      </c>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16">
+        <v>16.46735</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15">
+        <v>15.2303</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16">
+        <v>15.2303</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="14">
+        <v>8.0224499999999992</v>
+      </c>
+      <c r="D15" s="15">
+        <v>6.6300400000000002</v>
+      </c>
+      <c r="E15" s="15">
+        <v>10.94285</v>
+      </c>
+      <c r="F15" s="15">
+        <v>19.357900000000001</v>
+      </c>
+      <c r="G15" s="15">
+        <v>8.9395799999999994</v>
+      </c>
+      <c r="H15" s="15">
+        <v>10.1531</v>
+      </c>
+      <c r="I15" s="16">
+        <v>11.793333749999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="14">
+        <v>9.6301400000000008</v>
+      </c>
+      <c r="D16" s="15">
+        <v>10.1149</v>
+      </c>
+      <c r="E16" s="15">
+        <v>15.442399999999999</v>
+      </c>
+      <c r="F16" s="15">
+        <v>7.2748499999999998</v>
+      </c>
+      <c r="G16" s="15">
+        <v>14.4039</v>
+      </c>
+      <c r="H16" s="15">
+        <v>13.343400000000001</v>
+      </c>
+      <c r="I16" s="16">
+        <v>11.701598333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="14">
+        <v>9.7490299999999994</v>
+      </c>
+      <c r="D17" s="15">
+        <v>10.639699999999999</v>
+      </c>
+      <c r="E17" s="15">
+        <v>15.36</v>
+      </c>
+      <c r="F17" s="15">
+        <v>7.2275900000000002</v>
+      </c>
+      <c r="G17" s="15">
+        <v>13.9245</v>
+      </c>
+      <c r="H17" s="15">
+        <v>12.3736</v>
+      </c>
+      <c r="I17" s="16">
+        <v>11.545736666666665</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15">
+        <v>7.8972300000000004</v>
+      </c>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15">
+        <v>5.7200300000000004</v>
+      </c>
+      <c r="I18" s="16">
+        <v>6.8086300000000008</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C19" s="14">
         <v>4.0504699999999998</v>
       </c>
-      <c r="D9" s="15">
-        <v>4.3552099999999996</v>
-      </c>
-      <c r="E9" s="15">
-        <v>5.65693</v>
-      </c>
-      <c r="F9" s="15">
-        <v>7.5746200000000004</v>
-      </c>
-      <c r="G9" s="15">
+      <c r="D19" s="15">
+        <v>4.3078699999999994</v>
+      </c>
+      <c r="E19" s="15">
+        <v>4.5901449999999997</v>
+      </c>
+      <c r="F19" s="15">
+        <v>6.9780700000000007</v>
+      </c>
+      <c r="G19" s="15">
         <v>6.1369600000000002</v>
       </c>
-      <c r="H9" s="15">
-        <v>4.4875100000000003</v>
-      </c>
-      <c r="I9" s="16">
-        <v>5.3769499999999999</v>
+      <c r="H19" s="15">
+        <v>4.6874649999999995</v>
+      </c>
+      <c r="I19" s="16">
+        <v>5.1314529999999996</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B10" s="17" t="s">
+    <row r="20" spans="2:9">
+      <c r="B20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15">
+        <v>4.2819700000000003</v>
+      </c>
+      <c r="I20" s="16">
+        <v>4.2819700000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="18">
-        <v>3.7688299999999999</v>
-      </c>
-      <c r="D10" s="19">
+      <c r="C21" s="18">
+        <v>3.86246</v>
+      </c>
+      <c r="D21" s="19">
         <v>2.5402200000000001</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E21" s="19">
         <v>5.7587000000000002</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F21" s="19">
         <v>1.6008500000000001</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G21" s="19">
         <v>3.3304100000000001</v>
       </c>
-      <c r="H10" s="19">
+      <c r="H21" s="19">
         <v>5.0047800000000002</v>
       </c>
-      <c r="I10" s="20">
-        <v>3.6672983333333331</v>
+      <c r="I21" s="20">
+        <v>3.7085542857142859</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B11" s="21" t="s">
+    <row r="22" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B22" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22">
-        <v>8.3487000000000009</v>
-      </c>
-      <c r="D11" s="23">
-        <v>7.6427766666666672</v>
-      </c>
-      <c r="E11" s="23">
-        <v>10.363876666666666</v>
-      </c>
-      <c r="F11" s="23">
-        <v>9.5876900000000003</v>
-      </c>
-      <c r="G11" s="23">
-        <v>11.816623333333334</v>
-      </c>
-      <c r="H11" s="23">
-        <v>10.950396666666668</v>
-      </c>
-      <c r="I11" s="24">
-        <v>9.7850105555555551</v>
+      <c r="C22" s="22">
+        <v>12.679225625000001</v>
+      </c>
+      <c r="D22" s="23">
+        <v>11.583373333333334</v>
+      </c>
+      <c r="E22" s="23">
+        <v>14.843252666666668</v>
+      </c>
+      <c r="F22" s="23">
+        <v>14.326230666666667</v>
+      </c>
+      <c r="G22" s="23">
+        <v>18.951756666666665</v>
+      </c>
+      <c r="H22" s="23">
+        <v>15.880739444444442</v>
+      </c>
+      <c r="I22" s="24">
+        <v>14.726490638297873</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="16" spans="2:9" ht="15.75" thickBot="1"/>
-    <row r="17" ht="15.75" thickBot="1"/>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="I8:I10">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="D8:D10">
+  <conditionalFormatting pivot="1" sqref="C8:C21">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3556,7 +5658,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="E8:E10">
+  <conditionalFormatting pivot="1" sqref="D8:D21">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3568,7 +5670,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="F8:F10">
+  <conditionalFormatting pivot="1" sqref="E8:E21">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3580,7 +5682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="G8:G10">
+  <conditionalFormatting pivot="1" sqref="F8:F21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3592,7 +5694,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="H8:H10">
+  <conditionalFormatting pivot="1" sqref="G8:G21">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -3604,8 +5706,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="C8:C10">
+  <conditionalFormatting pivot="1" sqref="H8:H21">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="I8:I21">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Added TextMenuExample. Applied all necessary changes due to the changes of AndEngine. (99% Solved by a 'Organize Imports' CTRL + SHIFT + O).
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="2" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -87,9 +87,6 @@
     <t>HTC Legend</t>
   </si>
   <si>
-    <t>HTC Hero</t>
-  </si>
-  <si>
     <t>HTC Wildfire</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>HTC Dream (G1)</t>
+  </si>
+  <si>
+    <t>HTC Hero/Droid Eris</t>
   </si>
 </sst>
 </file>
@@ -277,25 +277,21 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -333,21 +329,480 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
+  <dxfs count="113">
+    <dxf>
+      <alignment textRotation="70" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment textRotation="70" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="medium">
@@ -901,13 +1356,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium16 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="60"/>
-      <tableStyleElement type="headerRow" dxfId="59"/>
-      <tableStyleElement type="totalRow" dxfId="58"/>
-      <tableStyleElement type="firstColumn" dxfId="57"/>
-      <tableStyleElement type="lastColumn" dxfId="56"/>
-      <tableStyleElement type="firstRowStripe" dxfId="55"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="54"/>
+      <tableStyleElement type="wholeTable" dxfId="112"/>
+      <tableStyleElement type="headerRow" dxfId="111"/>
+      <tableStyleElement type="totalRow" dxfId="110"/>
+      <tableStyleElement type="firstColumn" dxfId="109"/>
+      <tableStyleElement type="lastColumn" dxfId="108"/>
+      <tableStyleElement type="firstRowStripe" dxfId="107"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="106"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -1110,7 +1565,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1143,7 +1598,7 @@
                   <c:v>23.908349999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.916253333333335</c:v>
+                  <c:v>16.27948235294118</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13.451033333333333</c:v>
@@ -1164,7 +1619,7 @@
                   <c:v>8.0224499999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.0411799999999998</c:v>
+                  <c:v>4.3786849999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4.1948260000000008</c:v>
@@ -1238,7 +1693,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1271,7 +1726,7 @@
                   <c:v>24.684950000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.44964</c:v>
+                  <c:v>14.679947499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12.562760000000001</c:v>
@@ -1295,7 +1750,7 @@
                   <c:v>6.6300400000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1483999999999996</c:v>
+                  <c:v>4.6807549999999996</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4.2086016666666666</c:v>
@@ -1366,7 +1821,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1399,7 +1854,7 @@
                   <c:v>33.08175</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.632691666666663</c:v>
+                  <c:v>19.260721428571426</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>16.066425000000002</c:v>
@@ -1426,7 +1881,7 @@
                   <c:v>10.94285</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.4483600000000001</c:v>
+                  <c:v>6.0571299999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5.1309749999999994</c:v>
@@ -1494,7 +1949,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1527,7 +1982,7 @@
                   <c:v>24.061250000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.319880000000001</c:v>
+                  <c:v>17.695971249999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18.474033333333335</c:v>
@@ -1551,7 +2006,7 @@
                   <c:v>19.357900000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.1750499999999997</c:v>
+                  <c:v>6.6844199999999994</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6.5596500000000004</c:v>
@@ -1622,7 +2077,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1658,7 +2113,7 @@
                   <c:v>24.884699999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.143581818181818</c:v>
+                  <c:v>25.159076923076928</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19.113999999999997</c:v>
@@ -1682,7 +2137,7 @@
                   <c:v>9.6063899999999993</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.5549999999999997</c:v>
+                  <c:v>6.5297999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5.9314899999999993</c:v>
@@ -1753,7 +2208,7 @@
                   <c:v>Sony Ericsson x10i Mini</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HTC Hero</c:v>
+                  <c:v>HTC Hero/Droid Eris</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>HTC Dream (G1)</c:v>
@@ -1786,7 +2241,7 @@
                   <c:v>31.0808</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.381090909090911</c:v>
+                  <c:v>23.614115384615388</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18.772185714285715</c:v>
@@ -1807,7 +2262,7 @@
                   <c:v>9.4552849999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.4402100000000004</c:v>
+                  <c:v>5.2401400000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4.8121649999999994</c:v>
@@ -1830,25 +2285,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="89656320"/>
-        <c:axId val="89662208"/>
+        <c:axId val="91611904"/>
+        <c:axId val="91613440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89656320"/>
+        <c:axId val="91611904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89662208"/>
+        <c:crossAx val="91613440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89662208"/>
+        <c:axId val="91613440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1862,7 +2317,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89656320"/>
+        <c:crossAx val="91611904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1875,8 +2330,8 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.70000000000000062" r="0.70000000000000062" t="0.78740157499999996" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75000000000000011" l="0.25" r="0.25" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1885,16 +2340,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>99332</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>118381</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>180173</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>186417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>639535</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>81642</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>612320</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1917,14 +2372,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40365.94729178241" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="285">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40366.71772523148" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="304">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="21">
     <cacheField name="id" numFmtId="0" sqlType="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="298"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="317"/>
     </cacheField>
     <cacheField name="timestamp" numFmtId="0" sqlType="11">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-06T22:40:07"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-07T12:51:25"/>
     </cacheField>
     <cacheField name="benchmark_id" numFmtId="0" sqlType="4">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5" count="6">
@@ -1937,32 +2392,34 @@
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_versionname" numFmtId="0" sqlType="12">
-      <sharedItems count="8">
+      <sharedItems count="9">
         <s v="1.1.5"/>
         <s v="1.1.1"/>
         <s v="1.1.4"/>
         <s v="1.1.3"/>
         <s v="1.1.0"/>
         <s v="1.0.9"/>
+        <s v="1.1.6"/>
         <s v="" u="1"/>
         <s v="benchmark_versionname" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_versioncode" numFmtId="0" sqlType="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9" maxValue="15" count="6">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="9" maxValue="16" count="7">
         <n v="15"/>
         <n v="11"/>
         <n v="14"/>
         <n v="13"/>
         <n v="10"/>
         <n v="9"/>
+        <n v="16"/>
       </sharedItems>
     </cacheField>
     <cacheField name="benchmark_fps" numFmtId="0" sqlType="7">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.5669" maxValue="40.272399999999998"/>
     </cacheField>
     <cacheField name="device_model" numFmtId="0" sqlType="12">
-      <sharedItems count="27">
+      <sharedItems count="28">
         <s v="Nexus One"/>
         <s v="HTC Tattoo"/>
         <s v="T-Mobile G1"/>
@@ -1987,6 +2444,7 @@
         <s v="T-Mobile myTouch 3G"/>
         <s v="Hero"/>
         <s v="XT701"/>
+        <s v="Eris"/>
         <s v="" u="1"/>
         <s v="device_model" u="1"/>
         <s v="HTC Nexus One" u="1"/>
@@ -2059,7 +2517,7 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="device_device" numFmtId="0" sqlType="12">
-      <sharedItems count="19">
+      <sharedItems count="20">
         <s v="passion"/>
         <s v="bahamas"/>
         <s v="dream"/>
@@ -2079,10 +2537,11 @@
         <s v="hero"/>
         <s v="supersonic"/>
         <s v="choles"/>
+        <s v="desirec"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_product" numFmtId="0" sqlType="12">
-      <sharedItems count="27">
+      <sharedItems count="28">
         <s v="passion"/>
         <s v="htc_tattoo"/>
         <s v="kila"/>
@@ -2110,6 +2569,7 @@
         <s v="passion_vf"/>
         <s v="opal"/>
         <s v="choles"/>
+        <s v="htc_desirec"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_cpuabi" numFmtId="0" sqlType="12">
@@ -2119,7 +2579,7 @@
       </sharedItems>
     </cacheField>
     <cacheField name="device_board" numFmtId="0" sqlType="12">
-      <sharedItems count="17">
+      <sharedItems count="18">
         <s v="mahimahi"/>
         <s v="bahamas"/>
         <s v="trout"/>
@@ -2137,6 +2597,7 @@
         <s v="hero"/>
         <s v="supersonic"/>
         <s v="choles"/>
+        <s v="desirec"/>
       </sharedItems>
     </cacheField>
     <cacheField name="device_fingerprint" numFmtId="0" sqlType="12">
@@ -2158,31 +2619,32 @@
     </cacheField>
     <cacheField name="Device2" numFmtId="0" databaseField="0">
       <fieldGroup base="6">
-        <discretePr count="27">
+        <discretePr count="28">
           <x v="0"/>
           <x v="1"/>
-          <x v="20"/>
+          <x v="19"/>
           <x v="2"/>
           <x v="3"/>
+          <x v="17"/>
+          <x v="16"/>
           <x v="18"/>
           <x v="17"/>
-          <x v="19"/>
-          <x v="18"/>
           <x v="4"/>
           <x v="5"/>
           <x v="6"/>
           <x v="7"/>
           <x v="8"/>
-          <x v="18"/>
+          <x v="17"/>
           <x v="9"/>
           <x v="10"/>
           <x v="11"/>
+          <x v="19"/>
+          <x v="20"/>
+          <x v="12"/>
+          <x v="18"/>
           <x v="20"/>
           <x v="16"/>
-          <x v="12"/>
-          <x v="19"/>
-          <x v="16"/>
-          <x v="17"/>
+          <x v="20"/>
           <x v="13"/>
           <x v="14"/>
           <x v="15"/>
@@ -2204,11 +2666,11 @@
           <s v=""/>
           <s v="device_model"/>
           <s v="HTC Nexus One"/>
-          <s v="Gruppe1"/>
           <s v="Gruppe3"/>
           <s v="Gruppe2"/>
           <s v="Gruppe4"/>
           <s v="Gruppe5"/>
+          <s v="Gruppe1"/>
         </groupItems>
       </fieldGroup>
     </cacheField>
@@ -2217,7 +2679,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="285">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="304">
   <r>
     <n v="16"/>
     <d v="2010-07-02T17:08:17"/>
@@ -8488,11 +8950,429 @@
     <x v="0"/>
     <s v="012312005194100"/>
   </r>
+  <r>
+    <n v="299"/>
+    <d v="2010-07-07T08:13:42"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.7161900000000001"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="300"/>
+    <d v="2010-07-07T08:14:38"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.6658999999999997"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="301"/>
+    <d v="2010-07-07T08:15:13"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.2131100000000004"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="302"/>
+    <d v="2010-07-07T08:15:56"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.1937899999999999"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="303"/>
+    <d v="2010-07-07T08:16:37"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.5045999999999999"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="304"/>
+    <d v="2010-07-07T08:17:15"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.0400700000000001"/>
+    <x v="24"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="7"/>
+    <s v="ERD79"/>
+    <x v="19"/>
+    <x v="27"/>
+    <x v="1"/>
+    <x v="17"/>
+    <s v="verizon/htc_desirec/desirec/desirec:2.1/ERD79/165907:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A100001238E2CD"/>
+  </r>
+  <r>
+    <n v="305"/>
+    <d v="2010-07-07T10:10:45"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.326899999999998"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="306"/>
+    <d v="2010-07-07T10:11:09"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.121500000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="307"/>
+    <d v="2010-07-07T10:11:36"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.777900000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="308"/>
+    <d v="2010-07-07T10:11:58"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.824300000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="309"/>
+    <d v="2010-07-07T10:12:28"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="24.964200000000002"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="310"/>
+    <d v="2010-07-07T10:12:58"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="23.737200000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031032926"/>
+  </r>
+  <r>
+    <n v="311"/>
+    <d v="2010-07-07T11:15:02"/>
+    <x v="0"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="25.5244"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="312"/>
+    <d v="2010-07-07T11:15:22"/>
+    <x v="3"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="20.680499999999999"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="313"/>
+    <d v="2010-07-07T11:15:41"/>
+    <x v="1"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="26.936299999999999"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="314"/>
+    <d v="2010-07-07T11:17:11"/>
+    <x v="4"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="16.8063"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="315"/>
+    <d v="2010-07-07T11:18:17"/>
+    <x v="2"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="18.642299999999999"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="316"/>
+    <d v="2010-07-07T11:18:53"/>
+    <x v="5"/>
+    <x v="6"/>
+    <x v="6"/>
+    <n v="26.054300000000001"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="17"/>
+    <s v="EPE54B"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957030835139"/>
+  </r>
+  <r>
+    <n v="317"/>
+    <d v="2010-07-07T12:51:25"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.5105"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion/passion/mahimahi:2.2/FRF91/43546:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957031423729"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
   <location ref="B6:I26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -8509,26 +9389,27 @@
       </items>
     </pivotField>
     <pivotField name="Benchmark Version" axis="axisPage" showAll="0">
-      <items count="9">
+      <items count="10">
         <item x="2"/>
         <item x="3"/>
+        <item m="1" x="8"/>
         <item m="1" x="7"/>
-        <item m="1" x="6"/>
         <item x="0"/>
         <item x="1"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0" countASubtotal="1"/>
     <pivotField name="Device" axis="axisRow" showAll="0">
-      <items count="28">
+      <items count="29">
         <item x="17"/>
+        <item m="1" x="27"/>
         <item m="1" x="26"/>
         <item m="1" x="25"/>
-        <item m="1" x="24"/>
         <item sd="0" x="0"/>
         <item sd="0" x="1"/>
         <item x="2"/>
@@ -8552,6 +9433,7 @@
         <item x="21"/>
         <item x="22"/>
         <item x="23"/>
+        <item x="24"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -8602,7 +9484,6 @@
         <item sd="0" x="1"/>
         <item x="15"/>
         <item sd="0" x="9"/>
-        <item n="HTC Hero" sd="0" x="16"/>
         <item sd="0" x="6"/>
         <item n="Samsung Galaxy Spica" sd="0" x="10"/>
         <item n="Samsung Galaxy S" sd="0" x="3"/>
@@ -8612,10 +9493,11 @@
         <item x="14"/>
         <item n="HTC Incredible" sd="0" x="7"/>
         <item x="13"/>
-        <item n="Motorola XT720/701" sd="0" x="17"/>
-        <item n="Motorola Droid/Milestone" sd="0" x="18"/>
-        <item n="HTC Magic" sd="0" x="19"/>
-        <item n="HTC Dream (G1)" sd="0" x="20"/>
+        <item n="Motorola XT720/701" sd="0" x="16"/>
+        <item n="Motorola Droid/Milestone" sd="0" x="17"/>
+        <item n="HTC Magic" sd="0" x="18"/>
+        <item n="HTC Dream (G1)" sd="0" x="19"/>
+        <item n="HTC Hero/Droid Eris" sd="0" x="20"/>
       </items>
       <autoSortScope>
         <pivotArea dataOnly="0" outline="0" fieldPosition="0">
@@ -8634,7 +9516,7 @@
   </rowFields>
   <rowItems count="19">
     <i>
-      <x v="10"/>
+      <x v="9"/>
     </i>
     <i>
       <x v="2"/>
@@ -8643,31 +9525,28 @@
       <x v="1"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="7"/>
     </i>
     <i>
-      <x v="15"/>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i>
       <x v="17"/>
     </i>
     <i>
-      <x/>
+      <x v="6"/>
     </i>
     <i>
       <x v="11"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="7"/>
     </i>
     <i>
       <x v="20"/>
@@ -8676,10 +9555,13 @@
       <x v="19"/>
     </i>
     <i>
-      <x v="13"/>
+      <x v="18"/>
     </i>
     <i>
-      <x v="9"/>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i>
       <x v="4"/>
@@ -8725,168 +9607,231 @@
   <dataFields count="1">
     <dataField name="FPS" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
-  <formats count="54">
-    <format dxfId="53">
+  <formats count="53">
+    <format dxfId="105">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="52">
+    <format dxfId="104">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="103">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="102">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="101">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="100">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="99">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="98">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="97">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="96">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="94">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="93">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="92">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="91">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="90">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="89">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="88">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="87">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="86">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="84">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="82">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="81">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="79">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="78">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="77">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="76">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="75">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="74">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="73">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="72">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="71">
       <pivotArea field="6" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="18">
+    <format dxfId="70">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="69">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="68">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="67">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="66">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="65">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="64">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="63">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="62">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -8895,25 +9840,61 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="61">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
-            <x v="2"/>
+            <x v="17"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="60">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
-            <x v="1"/>
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="14">
+    <format dxfId="59">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="58">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="57">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="56">
+      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
+        <references count="1">
+          <reference field="20" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="55">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -8922,115 +9903,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="15"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="12">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="17"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="11">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="10">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="11"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="18"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="8">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="7">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="12"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="5">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="20"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="4">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="19"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="13"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="2">
-      <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
-        <references count="1">
-          <reference field="20" count="1">
-            <x v="9"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="1">
+    <format dxfId="54">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9039,7 +9912,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="0">
+    <format dxfId="53">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9058,7 +9931,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -9088,7 +9961,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -9098,7 +9971,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -9108,7 +9981,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -9128,7 +10001,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -9138,7 +10011,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -9158,7 +10031,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -9168,7 +10041,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -9178,7 +10051,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -9188,7 +10061,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -9198,7 +10071,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -9208,7 +10081,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -9245,7 +10118,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -9284,7 +10157,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -9297,7 +10170,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -9310,7 +10183,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -9336,7 +10209,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -9349,7 +10222,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -9375,7 +10248,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -9388,7 +10261,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -9401,7 +10274,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -9414,7 +10287,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -9427,7 +10300,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -9440,7 +10313,7 @@
               <x v="5"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -9483,7 +10356,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -9522,7 +10395,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -9535,7 +10408,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -9548,7 +10421,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -9574,7 +10447,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -9587,7 +10460,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -9613,7 +10486,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -9626,7 +10499,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -9639,7 +10512,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -9652,7 +10525,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -9665,7 +10538,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -9678,7 +10551,7 @@
               <x v="4"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -9721,7 +10594,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -9760,7 +10633,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -9773,7 +10646,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -9786,7 +10659,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -9812,7 +10685,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -9825,7 +10698,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -9851,7 +10724,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -9864,7 +10737,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -9877,7 +10750,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -9890,7 +10763,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -9903,7 +10776,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -9916,7 +10789,7 @@
               <x v="3"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -9959,7 +10832,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -9998,7 +10871,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -10011,7 +10884,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -10024,7 +10897,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -10050,7 +10923,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -10063,7 +10936,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -10089,7 +10962,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -10102,7 +10975,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -10115,7 +10988,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -10128,7 +11001,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -10141,7 +11014,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -10154,7 +11027,7 @@
               <x v="2"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -10197,7 +11070,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -10236,7 +11109,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -10249,7 +11122,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -10262,7 +11135,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -10288,7 +11161,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -10301,7 +11174,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -10327,7 +11200,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -10340,7 +11213,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -10353,7 +11226,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -10366,7 +11239,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -10379,7 +11252,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -10392,7 +11265,7 @@
               <x v="1"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -10435,7 +11308,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="10"/>
+              <x v="9"/>
             </reference>
           </references>
         </pivotArea>
@@ -10474,7 +11347,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="8"/>
+              <x v="7"/>
             </reference>
           </references>
         </pivotArea>
@@ -10487,7 +11360,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="15"/>
+              <x v="14"/>
             </reference>
           </references>
         </pivotArea>
@@ -10500,7 +11373,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="17"/>
+              <x v="16"/>
             </reference>
           </references>
         </pivotArea>
@@ -10526,7 +11399,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="11"/>
+              <x v="10"/>
             </reference>
           </references>
         </pivotArea>
@@ -10539,7 +11412,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="18"/>
+              <x v="17"/>
             </reference>
           </references>
         </pivotArea>
@@ -10565,7 +11438,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="12"/>
+              <x v="11"/>
             </reference>
           </references>
         </pivotArea>
@@ -10578,7 +11451,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="7"/>
+              <x v="20"/>
             </reference>
           </references>
         </pivotArea>
@@ -10591,7 +11464,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="20"/>
+              <x v="19"/>
             </reference>
           </references>
         </pivotArea>
@@ -10604,7 +11477,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="19"/>
+              <x v="18"/>
             </reference>
           </references>
         </pivotArea>
@@ -10617,7 +11490,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="13"/>
+              <x v="12"/>
             </reference>
           </references>
         </pivotArea>
@@ -10630,7 +11503,7 @@
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
-              <x v="9"/>
+              <x v="8"/>
             </reference>
           </references>
         </pivotArea>
@@ -11121,8 +11994,8 @@
   </sheetPr>
   <dimension ref="B2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11130,12 +12003,7 @@
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
     <col min="3" max="9" width="7.140625" customWidth="1"/>
-    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5703125" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="17" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9">
@@ -11204,8 +12072,8 @@
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="23" t="s">
-        <v>23</v>
+      <c r="B8" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="9">
         <v>23.908349999999999</v>
@@ -11230,8 +12098,8 @@
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="23" t="s">
-        <v>22</v>
+      <c r="B9" s="22" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
@@ -11246,33 +12114,33 @@
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="11">
-        <v>15.916253333333335</v>
+        <v>16.27948235294118</v>
       </c>
       <c r="D10" s="12">
-        <v>14.44964</v>
+        <v>14.679947499999999</v>
       </c>
       <c r="E10" s="12">
-        <v>18.632691666666663</v>
+        <v>19.260721428571426</v>
       </c>
       <c r="F10" s="12">
-        <v>17.319880000000001</v>
+        <v>17.695971249999999</v>
       </c>
       <c r="G10" s="12">
-        <v>25.143581818181818</v>
+        <v>25.159076923076928</v>
       </c>
       <c r="H10" s="12">
-        <v>23.381090909090911</v>
+        <v>23.614115384615388</v>
       </c>
       <c r="I10" s="20">
-        <v>18.731064473684217</v>
+        <v>19.083904494382026</v>
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="11">
@@ -11298,8 +12166,8 @@
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="23" t="s">
-        <v>24</v>
+      <c r="B12" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="11">
         <v>13.2644</v>
@@ -11324,8 +12192,8 @@
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="23" t="s">
-        <v>25</v>
+      <c r="B13" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="11">
         <v>12.5755</v>
@@ -11350,8 +12218,8 @@
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="23" t="s">
-        <v>26</v>
+      <c r="B14" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="11">
         <v>13.298999999999999</v>
@@ -11372,8 +12240,8 @@
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="23" t="s">
-        <v>30</v>
+      <c r="B15" s="22" t="s">
+        <v>29</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="12">
@@ -11392,8 +12260,8 @@
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="23" t="s">
-        <v>29</v>
+      <c r="B16" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="11">
         <v>10.060796666666667</v>
@@ -11418,7 +12286,7 @@
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="11"/>
@@ -11440,8 +12308,8 @@
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="23" t="s">
-        <v>27</v>
+      <c r="B18" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="11">
         <v>8.0224499999999992</v>
@@ -11466,34 +12334,34 @@
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="23" t="s">
-        <v>20</v>
+      <c r="B19" s="22" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="11">
-        <v>5.0411799999999998</v>
+        <v>4.3786849999999999</v>
       </c>
       <c r="D19" s="12">
-        <v>5.1483999999999996</v>
+        <v>4.6807549999999996</v>
       </c>
       <c r="E19" s="12">
-        <v>6.4483600000000001</v>
+        <v>6.0571299999999999</v>
       </c>
       <c r="F19" s="12">
-        <v>6.1750499999999997</v>
+        <v>6.6844199999999994</v>
       </c>
       <c r="G19" s="12">
-        <v>6.5549999999999997</v>
+        <v>6.5297999999999998</v>
       </c>
       <c r="H19" s="12">
-        <v>5.4402100000000004</v>
-      </c>
-      <c r="I19" s="20">
-        <v>5.8013666666666666</v>
+        <v>5.2401400000000002</v>
+      </c>
+      <c r="I19" s="23">
+        <v>5.595155000000001</v>
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="23" t="s">
-        <v>31</v>
+      <c r="B20" s="22" t="s">
+        <v>30</v>
       </c>
       <c r="C20" s="11">
         <v>4.1948260000000008</v>
@@ -11518,7 +12386,7 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="22" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="11">
@@ -11540,7 +12408,7 @@
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="11"/>
@@ -11556,8 +12424,8 @@
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="23" t="s">
-        <v>28</v>
+      <c r="B23" s="22" t="s">
+        <v>27</v>
       </c>
       <c r="C23" s="11">
         <v>2.38863</v>
@@ -11582,7 +12450,7 @@
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="11">
@@ -11608,8 +12476,8 @@
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B25" s="23" t="s">
-        <v>21</v>
+      <c r="B25" s="22" t="s">
+        <v>20</v>
       </c>
       <c r="C25" s="11">
         <v>3.1853899999999999</v>
@@ -11621,7 +12489,7 @@
         <v>3.0426899999999999</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="21">
+      <c r="I25" s="20">
         <v>3.1140400000000001</v>
       </c>
     </row>
@@ -11630,30 +12498,31 @@
         <v>7</v>
       </c>
       <c r="C26" s="14">
-        <v>11.300381458333332</v>
+        <v>11.453762745098034</v>
       </c>
       <c r="D26" s="15">
-        <v>10.39603224489796</v>
+        <v>10.503901730769231</v>
       </c>
       <c r="E26" s="15">
-        <v>14.814152978723401</v>
+        <v>14.959777799999998</v>
       </c>
       <c r="F26" s="15">
-        <v>12.369192553191493</v>
+        <v>12.676920392156864</v>
       </c>
       <c r="G26" s="15">
-        <v>16.888563043478264</v>
+        <v>17.017695918367352</v>
       </c>
       <c r="H26" s="15">
-        <v>15.581374999999994</v>
-      </c>
-      <c r="I26" s="22">
-        <v>13.523582561403508</v>
+        <v>15.739952352941172</v>
+      </c>
+      <c r="I26" s="21">
+        <v>13.689017401315789</v>
       </c>
     </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="53" ht="15.75" thickBot="1"/>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25">
+  <conditionalFormatting pivot="1" sqref="C9 C8 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11677,7 +12546,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25">
+  <conditionalFormatting pivot="1" sqref="E9 E8 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11701,7 +12570,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25">
+  <conditionalFormatting pivot="1" sqref="G9 G8 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11725,7 +12594,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="I8 I9 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25">
+  <conditionalFormatting pivot="1" sqref="I9 I8 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -11737,8 +12606,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed version number - now correct.
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -159,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -198,17 +198,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -294,520 +283,213 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="70"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="113">
-    <dxf>
-      <alignment textRotation="70" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment textRotation="70" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="78">
     <dxf>
       <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
     </dxf>
     <dxf>
       <border>
         <right style="medium">
           <color indexed="64"/>
         </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
       <border>
-        <left style="medium">
+        <right style="medium">
           <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
+        </right>
       </border>
     </dxf>
     <dxf>
@@ -1356,13 +1038,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleMedium16 2" pivot="0" count="7">
-      <tableStyleElement type="wholeTable" dxfId="112"/>
-      <tableStyleElement type="headerRow" dxfId="111"/>
-      <tableStyleElement type="totalRow" dxfId="110"/>
-      <tableStyleElement type="firstColumn" dxfId="109"/>
-      <tableStyleElement type="lastColumn" dxfId="108"/>
-      <tableStyleElement type="firstRowStripe" dxfId="107"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="106"/>
+      <tableStyleElement type="wholeTable" dxfId="77"/>
+      <tableStyleElement type="headerRow" dxfId="76"/>
+      <tableStyleElement type="totalRow" dxfId="75"/>
+      <tableStyleElement type="firstColumn" dxfId="74"/>
+      <tableStyleElement type="lastColumn" dxfId="73"/>
+      <tableStyleElement type="firstRowStripe" dxfId="72"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="71"/>
     </tableStyle>
   </tableStyles>
 </styleSheet>
@@ -2285,25 +1967,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="91611904"/>
-        <c:axId val="91613440"/>
+        <c:axId val="88314624"/>
+        <c:axId val="88316160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91611904"/>
+        <c:axId val="88314624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91613440"/>
+        <c:crossAx val="88316160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91613440"/>
+        <c:axId val="88316160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +1999,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91611904"/>
+        <c:crossAx val="88314624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2330,7 +2012,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.25" r="0.25" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.25" r="0.25" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -9372,7 +9054,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Benchmarks" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" grandTotalCaption="Average" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1" rowHeaderCaption="Device" colHeaderCaption="Bench" fieldListSortAscending="1">
   <location ref="B6:I26" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="21">
     <pivotField showAll="0"/>
@@ -9607,168 +9289,168 @@
   <dataFields count="1">
     <dataField name="FPS" fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
-  <formats count="53">
-    <format dxfId="105">
+  <formats count="71">
+    <format dxfId="70">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="104">
+    <format dxfId="69">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="103">
+    <format dxfId="68">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="67">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="101">
+    <format dxfId="66">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="65">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="99">
+    <format dxfId="64">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="98">
+    <format dxfId="63">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="97">
+    <format dxfId="62">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="61">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="95">
+    <format dxfId="60">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="59">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="93">
+    <format dxfId="58">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="92">
+    <format dxfId="57">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="56">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="55">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="89">
+    <format dxfId="54">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="88">
+    <format dxfId="53">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="87">
+    <format dxfId="52">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="51">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="85">
+    <format dxfId="50">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="84">
+    <format dxfId="49">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="48">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="82">
+    <format dxfId="47">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="81">
+    <format dxfId="46">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="45">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="3" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="79">
+    <format dxfId="44">
       <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="1"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="43">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="9" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="42">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="2"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="41">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="7" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="75">
+    <format dxfId="40">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="39">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="38">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="37">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="36">
       <pivotArea field="6" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="1">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="70">
+    <format dxfId="35">
       <pivotArea grandRow="1" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="69">
+    <format dxfId="34">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9777,7 +9459,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="68">
+    <format dxfId="33">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9786,7 +9468,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="32">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9795,7 +9477,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="66">
+    <format dxfId="31">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9804,7 +9486,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="30">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9813,7 +9495,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="29">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9822,7 +9504,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="28">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9831,7 +9513,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="27">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9840,7 +9522,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="61">
+    <format dxfId="26">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9849,7 +9531,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="60">
+    <format dxfId="25">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9858,7 +9540,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="59">
+    <format dxfId="24">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9867,7 +9549,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="23">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9876,7 +9558,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="57">
+    <format dxfId="22">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9885,7 +9567,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="56">
+    <format dxfId="21">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9894,7 +9576,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="55">
+    <format dxfId="20">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9903,7 +9585,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="19">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9912,7 +9594,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="53">
+    <format dxfId="18">
       <pivotArea field="20" grandCol="1" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="20" count="1">
@@ -9921,13 +9603,196 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="17">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="16">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="13">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="14"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="16"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="11">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="10">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="17"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="8">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="7">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="11"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="20"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="19"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="4">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="18"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="12"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="2">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="1">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="2" count="0" selected="0"/>
+          <reference field="20" count="1">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
   </formats>
   <conditionalFormats count="7">
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="7">
       <pivotAreas count="18">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9935,9 +9800,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9945,9 +9813,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9955,9 +9826,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9965,9 +9839,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9975,9 +9852,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -9985,19 +9865,25 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10005,9 +9891,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10015,9 +9904,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10025,9 +9917,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10035,9 +9930,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10045,9 +9943,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10055,9 +9956,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10065,9 +9969,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10075,9 +9982,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10085,9 +9995,12 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -10095,10 +10008,965 @@
             </reference>
           </references>
         </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="6">
+      <pivotAreas count="18">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="14"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="1"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="5">
+      <pivotAreas count="18">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="14"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="2"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="4">
+      <pivotAreas count="18">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="14"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="3"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="3">
+      <pivotAreas count="18">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="14"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="2" count="1" selected="0">
+              <x v="4"/>
             </reference>
             <reference field="20" count="1">
               <x v="3"/>
@@ -10345,1187 +11213,181 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="1">
       <pivotAreas count="18">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="14"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="12"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
               <x v="4"/>
             </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="14"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="12"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="4"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="4">
-      <pivotAreas count="18">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="14"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="12"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="3"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="5">
-      <pivotAreas count="18">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="14"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="12"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="2"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="6">
-      <pivotAreas count="18">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="14"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="12"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="1"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="7">
-      <pivotAreas count="18">
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="14"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="12"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="3">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="2" count="1" selected="0">
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
               <x v="0"/>
             </reference>
             <reference field="20" count="1">
@@ -11995,7 +11857,7 @@
   <dimension ref="B2:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E19:E20"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12072,7 +11934,7 @@
       </c>
     </row>
     <row r="8" spans="2:9">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="20" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="9">
@@ -12090,15 +11952,15 @@
       <c r="G8" s="10">
         <v>33.013099999999994</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="22">
         <v>31.0808</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="22">
         <v>28.305033333333331</v>
       </c>
     </row>
     <row r="9" spans="2:9">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="20" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="11"/>
@@ -12108,13 +11970,13 @@
       <c r="G9" s="12">
         <v>24.884699999999999</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="20">
+      <c r="H9" s="21"/>
+      <c r="I9" s="21">
         <v>24.884699999999999</v>
       </c>
     </row>
     <row r="10" spans="2:9">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="11">
@@ -12132,15 +11994,15 @@
       <c r="G10" s="12">
         <v>25.159076923076928</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="21">
         <v>23.614115384615388</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="21">
         <v>19.083904494382026</v>
       </c>
     </row>
     <row r="11" spans="2:9">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="11">
@@ -12158,15 +12020,15 @@
       <c r="G11" s="12">
         <v>19.113999999999997</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="21">
         <v>18.772185714285715</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="21">
         <v>16.660370370370369</v>
       </c>
     </row>
     <row r="12" spans="2:9">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="11">
@@ -12184,15 +12046,15 @@
       <c r="G12" s="12">
         <v>17.847966666666668</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="21">
         <v>20.0868</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="21">
         <v>15.887011764705884</v>
       </c>
     </row>
     <row r="13" spans="2:9">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="20" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="11">
@@ -12210,15 +12072,15 @@
       <c r="G13" s="12">
         <v>14.9398</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="21">
         <v>25.3642</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="21">
         <v>15.206027142857142</v>
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="11">
@@ -12234,13 +12096,13 @@
       <c r="G14" s="12">
         <v>18.615500000000001</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="20">
+      <c r="H14" s="21"/>
+      <c r="I14" s="21">
         <v>13.702695</v>
       </c>
     </row>
     <row r="15" spans="2:9">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="11"/>
@@ -12254,13 +12116,13 @@
         <v>10.795299999999999</v>
       </c>
       <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="20">
+      <c r="H15" s="21"/>
+      <c r="I15" s="21">
         <v>12.264499999999998</v>
       </c>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="11">
@@ -12278,15 +12140,15 @@
       <c r="G16" s="12">
         <v>14.520400000000002</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="21">
         <v>13.645518181818181</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="21">
         <v>11.946854999999998</v>
       </c>
     </row>
     <row r="17" spans="2:9">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="11"/>
@@ -12300,15 +12162,15 @@
       <c r="G17" s="12">
         <v>9.7563449999999996</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="21">
         <v>7.8437000000000001</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="21">
         <v>11.795909999999999</v>
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="11">
@@ -12326,15 +12188,15 @@
       <c r="G18" s="12">
         <v>9.6063899999999993</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="21">
         <v>9.4552849999999999</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="21">
         <v>11.337733999999999</v>
       </c>
     </row>
     <row r="19" spans="2:9">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="20" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="11">
@@ -12352,15 +12214,15 @@
       <c r="G19" s="12">
         <v>6.5297999999999998</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="21">
         <v>5.2401400000000002</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="21">
         <v>5.595155000000001</v>
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="11">
@@ -12378,15 +12240,15 @@
       <c r="G20" s="12">
         <v>5.9314899999999993</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="21">
         <v>4.8121649999999994</v>
       </c>
-      <c r="I20" s="20">
+      <c r="I20" s="21">
         <v>5.0589266666666663</v>
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="20" t="s">
         <v>17</v>
       </c>
       <c r="C21" s="11">
@@ -12400,15 +12262,15 @@
         <v>5.8046433333333338</v>
       </c>
       <c r="G21" s="12"/>
-      <c r="H21" s="12">
+      <c r="H21" s="21">
         <v>5.7200300000000004</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I21" s="21">
         <v>4.8550966666666673</v>
       </c>
     </row>
     <row r="22" spans="2:9">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C22" s="11"/>
@@ -12416,15 +12278,15 @@
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
-      <c r="H22" s="12">
+      <c r="H22" s="21">
         <v>4.2819700000000003</v>
       </c>
-      <c r="I22" s="20">
+      <c r="I22" s="21">
         <v>4.2819700000000003</v>
       </c>
     </row>
     <row r="23" spans="2:9">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="20" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="11">
@@ -12442,15 +12304,15 @@
       <c r="G23" s="12">
         <v>4.5509500000000003</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="21">
         <v>5.0518850000000004</v>
       </c>
-      <c r="I23" s="20">
+      <c r="I23" s="21">
         <v>3.86794875</v>
       </c>
     </row>
     <row r="24" spans="2:9">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="20" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="11">
@@ -12468,28 +12330,28 @@
       <c r="G24" s="12">
         <v>3.3733599999999999</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="21">
         <v>4.9798450000000001</v>
       </c>
-      <c r="I24" s="20">
+      <c r="I24" s="21">
         <v>3.6049100000000003</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="15.75" thickBot="1">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="23">
         <v>3.1853899999999999</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12">
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24">
         <v>3.0426899999999999</v>
       </c>
-      <c r="H25" s="12"/>
-      <c r="I25" s="20">
+      <c r="H25" s="25"/>
+      <c r="I25" s="21">
         <v>3.1140400000000001</v>
       </c>
     </row>
@@ -12515,14 +12377,14 @@
       <c r="H26" s="15">
         <v>15.739952352941172</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="19">
         <v>13.689017401315789</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="15.75" thickBot="1"/>
     <row r="53" ht="15.75" thickBot="1"/>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="C9 C8 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25">
+  <conditionalFormatting pivot="1" sqref="C8 C9 C10 C11 C12 C13 C14 C15 C16 C17 C18 C19 C20 C21 C22 C23 C24 C25">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12534,7 +12396,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="D9 D8 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25">
+  <conditionalFormatting pivot="1" sqref="D8 D9 D10 D11 D12 D13 D14 D15 D16 D17 D18 D19 D20 D21 D22 D23 D24 D25">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12546,7 +12408,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="E9 E8 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25">
+  <conditionalFormatting pivot="1" sqref="E8 E9 E10 E11 E12 E13 E14 E15 E16 E17 E18 E19 E20 E21 E22 E23 E24 E25">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12558,7 +12420,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="F9 F8 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25">
+  <conditionalFormatting pivot="1" sqref="F8 F9 F10 F11 F12 F13 F14 F15 F16 F17 F18 F19 F20 F21 F22 F23 F24 F25">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12570,7 +12432,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="G9 G8 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25">
+  <conditionalFormatting pivot="1" sqref="G8 G9 G10 G11 G12 G13 G14 G15 G16 G17 G18 G19 G20 G21 G22 G23 G24 G25">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12582,7 +12444,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="H9 H8 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25">
+  <conditionalFormatting pivot="1" sqref="H8 H9 H10 H11 H12 H13 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -12594,7 +12456,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="I9 I8 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25">
+  <conditionalFormatting pivot="1" sqref="I8 I9 I10 I11 I12 I13 I14 I15 I16 I17 I18 I19 I20 I21 I22 I23 I24 I25">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>

</xml_diff>

<commit_message>
Updated andengine.jar. Updated andenginephysicsbox2dextenion stuff. Updated Benchmarks.
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -2351,10 +2351,10 @@
                   <c:v>22.560333333333332</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.563800000000001</c:v>
+                  <c:v>20.417250000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.872334285714288</c:v>
+                  <c:v>15.907547222222226</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.500866666666667</c:v>
@@ -2378,7 +2378,7 @@
                   <c:v>11.35102</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.410885454545454</c:v>
+                  <c:v>10.385745217391305</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>7.0424699999999998</c:v>
@@ -2527,10 +2527,10 @@
                   <c:v>22.389366666666671</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.592350000000003</c:v>
+                  <c:v>20.314333333333334</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.462973448275861</c:v>
+                  <c:v>14.501937666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10.2979425</c:v>
@@ -2542,7 +2542,7 @@
                   <c:v>12.408959999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.717436153846153</c:v>
+                  <c:v>11.745934814814813</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>10.3766</c:v>
@@ -2554,7 +2554,7 @@
                   <c:v>10.4309625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.320928571428572</c:v>
+                  <c:v>10.332336363636365</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>6.9973299999999998</c:v>
@@ -2572,7 +2572,7 @@
                   <c:v>5.6898900000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.9067046153846148</c:v>
+                  <c:v>4.8980499999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>4.2856888888888882</c:v>
@@ -2703,10 +2703,10 @@
                   <c:v>31.863499999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.5059</c:v>
+                  <c:v>29.591566666666665</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.671042307692304</c:v>
+                  <c:v>18.689214814814811</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>15.815133333333334</c:v>
@@ -2715,7 +2715,7 @@
                   <c:v>15.877516666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.669700000000002</c:v>
+                  <c:v>15.685662500000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>17.708550000000002</c:v>
@@ -2724,7 +2724,7 @@
                   <c:v>14.146700000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.388391666666667</c:v>
+                  <c:v>16.313532000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>11.0708</c:v>
@@ -2742,7 +2742,7 @@
                   <c:v>11.763299999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.4911266666666663</c:v>
+                  <c:v>6.2352729999999994</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5.405804285714285</c:v>
@@ -2867,10 +2867,10 @@
                   <c:v>20.887150000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.869499999999999</c:v>
+                  <c:v>16.808974999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.553158571428575</c:v>
+                  <c:v>18.589053103448279</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>22.698499999999999</c:v>
@@ -2888,7 +2888,7 @@
                   <c:v>15.963666666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2259175000000013</c:v>
+                  <c:v>7.2235847619047631</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>24.994299999999999</c:v>
@@ -3031,10 +3031,10 @@
                   <c:v>26.762649999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.144649999999999</c:v>
+                  <c:v>27.345933333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.065959259259259</c:v>
+                  <c:v>24.107971428571428</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20.30885</c:v>
@@ -3058,7 +3058,7 @@
                   <c:v>16.103333333333335</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.949708695652173</c:v>
+                  <c:v>14.895436</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>11.183199999999999</c:v>
@@ -3076,13 +3076,13 @@
                   <c:v>10.223100000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.773477777777777</c:v>
+                  <c:v>6.7621349999999989</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>5.7307522222222227</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.9323874999999999</c:v>
+                  <c:v>6.0004140000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>4.2554266666666667</c:v>
@@ -3204,10 +3204,10 @@
                   <c:v>30.769728571428573</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.66375</c:v>
+                  <c:v>25.632200000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22.488084848484849</c:v>
+                  <c:v>22.388105882352942</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>20.806066666666666</c:v>
@@ -3216,7 +3216,7 @@
                   <c:v>20.301440000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.950385294117641</c:v>
+                  <c:v>18.984417142857136</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>25.3642</c:v>
@@ -3225,7 +3225,7 @@
                   <c:v>16.1661</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>14.630042307692309</c:v>
+                  <c:v>14.576396296296297</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>9.8284500000000001</c:v>
@@ -3243,10 +3243,10 @@
                   <c:v>8.0161899999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9769220000000001</c:v>
+                  <c:v>5.9464333333333341</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.5478739999999993</c:v>
+                  <c:v>4.5124054545454539</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>4.7087199999999996</c:v>
@@ -3269,25 +3269,25 @@
         </c:ser>
         <c:gapWidth val="75"/>
         <c:overlap val="100"/>
-        <c:axId val="87116800"/>
-        <c:axId val="87143168"/>
+        <c:axId val="52648960"/>
+        <c:axId val="52675328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="87116800"/>
+        <c:axId val="52648960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87143168"/>
+        <c:crossAx val="52675328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87143168"/>
+        <c:axId val="52675328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3319,7 +3319,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87116800"/>
+        <c:crossAx val="52648960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3332,7 +3332,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.25" r="0.25" t="0.75000000000000033" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000044" l="0.25" r="0.25" t="0.75000000000000044" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -3374,14 +3374,14 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40381.832257175927" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="834">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="nico" refreshedDate="40382.877015393518" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="864">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="21">
     <cacheField name="id" numFmtId="0" sqlType="4">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="848"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12" maxValue="878"/>
     </cacheField>
     <cacheField name="timestamp" numFmtId="0" sqlType="11">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-22T19:51:04"/>
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2010-07-02T17:05:18" maxDate="2010-07-23T13:02:52"/>
     </cacheField>
     <cacheField name="benchmark_id" numFmtId="0" sqlType="4">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="5" count="6">
@@ -3687,7 +3687,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="834">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="864">
   <r>
     <n v="16"/>
     <d v="2010-07-02T17:08:17"/>
@@ -22035,6 +22035,666 @@
     <x v="0"/>
     <x v="0"/>
     <s v="A100001350357F"/>
+  </r>
+  <r>
+    <n v="849"/>
+    <d v="2010-07-22T21:58:07"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="20.141500000000001"/>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="11"/>
+    <s v="htc_bravo"/>
+    <x v="0"/>
+    <x v="8"/>
+    <s v="htc_wwe/htc_bravo/bravo/bravo:2.1-update1/ERE27/174215:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357841035326699"/>
+  </r>
+  <r>
+    <n v="850"/>
+    <d v="2010-07-22T21:58:26"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.052800000000001"/>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="11"/>
+    <s v="htc_bravo"/>
+    <x v="0"/>
+    <x v="8"/>
+    <s v="htc_wwe/htc_bravo/bravo/bravo:2.1-update1/ERE27/174215:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357841035326699"/>
+  </r>
+  <r>
+    <n v="851"/>
+    <d v="2010-07-22T21:58:43"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="12.4869"/>
+    <x v="11"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="11"/>
+    <s v="htc_bravo"/>
+    <x v="0"/>
+    <x v="8"/>
+    <s v="htc_wwe/htc_bravo/bravo/bravo:2.1-update1/ERE27/174215:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="357841035326699"/>
+  </r>
+  <r>
+    <n v="852"/>
+    <d v="2010-07-22T22:49:27"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.1577200000000003"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="DMD64"/>
+    <s v="DMD64"/>
+    <x v="2"/>
+    <s v="kila"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="tmobile/kila/dream/trout:1.6/DMD64/21415:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="351680031121373"/>
+  </r>
+  <r>
+    <n v="853"/>
+    <d v="2010-07-23T01:59:16"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="9.8326600000000006"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="854"/>
+    <d v="2010-07-23T01:59:38"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.5169"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="855"/>
+    <d v="2010-07-23T01:59:59"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="10.571899999999999"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="856"/>
+    <d v="2010-07-23T02:00:19"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="7.1769299999999996"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="857"/>
+    <d v="2010-07-23T02:00:58"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.301600000000001"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="858"/>
+    <d v="2010-07-23T02:01:29"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="13.1816"/>
+    <x v="5"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="ESE81"/>
+    <s v="ESE81"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.1-update1/ESE81/29593:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000015BBD3D3"/>
+  </r>
+  <r>
+    <n v="859"/>
+    <d v="2010-07-23T02:14:27"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.2725200000000001"/>
+    <x v="7"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="EPE54B"/>
+    <s v="EPE54B"/>
+    <x v="7"/>
+    <s v="opal"/>
+    <x v="1"/>
+    <x v="6"/>
+    <s v="google/passion/passion/mahimahi:2.1-update1/ERE27/24178:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="352949030311304"/>
+  </r>
+  <r>
+    <n v="860"/>
+    <d v="2010-07-23T02:39:46"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.69015"/>
+    <x v="19"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="htc_rus/htc_hero/hero/hero:2.1-update1/ERE27/191507:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357988022896273"/>
+  </r>
+  <r>
+    <n v="861"/>
+    <d v="2010-07-23T02:40:13"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.97302"/>
+    <x v="19"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="htc_rus/htc_hero/hero/hero:2.1-update1/ERE27/191507:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="357988022896273"/>
+  </r>
+  <r>
+    <n v="862"/>
+    <d v="2010-07-23T04:02:58"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="29.762899999999998"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="863"/>
+    <d v="2010-07-23T04:03:26"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.758299999999998"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="864"/>
+    <d v="2010-07-23T04:03:51"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="21.270700000000001"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="865"/>
+    <d v="2010-07-23T04:04:15"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="16.627400000000002"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="866"/>
+    <d v="2010-07-23T04:04:48"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="27.7485"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="867"/>
+    <d v="2010-07-23T04:05:16"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.569099999999999"/>
+    <x v="34"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="3"/>
+    <s v="VZW"/>
+    <s v="VZW"/>
+    <x v="26"/>
+    <s v="shadow_vzw"/>
+    <x v="0"/>
+    <x v="24"/>
+    <s v="verizon/shadow_vzw/cdma_shadow/shadow:2.1-update1/VZW/13604:user/ota-rel-keys,release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A0000022426B22"/>
+  </r>
+  <r>
+    <n v="868"/>
+    <d v="2010-07-23T09:21:53"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="14.241"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="3"/>
+    <s v="FRF84B"/>
+    <s v="FRF84B"/>
+    <x v="5"/>
+    <s v="voles"/>
+    <x v="0"/>
+    <x v="5"/>
+    <s v="verizon/voles/sholes/sholes:2.2/FRF84B/42477:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="A000002202E499"/>
+  </r>
+  <r>
+    <n v="869"/>
+    <d v="2010-07-23T10:05:23"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.9325899999999998"/>
+    <x v="19"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="HTC/htc_hero/hero/hero:2.1-update1/ERE27/183682:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357988027465033"/>
+  </r>
+  <r>
+    <n v="870"/>
+    <d v="2010-07-23T10:50:52"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="17.14"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="871"/>
+    <d v="2010-07-23T10:51:09"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.1617"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="872"/>
+    <d v="2010-07-23T10:51:27"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="15.6319"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="873"/>
+    <d v="2010-07-23T10:51:46"/>
+    <x v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.594100000000001"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="874"/>
+    <d v="2010-07-23T10:52:11"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="25.2423"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="875"/>
+    <d v="2010-07-23T10:52:39"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="19.088799999999999"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="FRF91"/>
+    <s v="FRF91"/>
+    <x v="0"/>
+    <s v="passion_vf"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="google/passion_vf/passion/mahimahi:2.2/FRF91/209740:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="354957032818422"/>
+  </r>
+  <r>
+    <n v="876"/>
+    <d v="2010-07-23T13:00:35"/>
+    <x v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.7105699999999997"/>
+    <x v="19"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="chunghwa/htc_hero/hero/hero:2.1-update1/ERE27/183682:user/release-keys"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="357988021213397"/>
+  </r>
+  <r>
+    <n v="877"/>
+    <d v="2010-07-23T13:01:08"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.66005"/>
+    <x v="19"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="chunghwa/htc_hero/hero/hero:2.1-update1/ERE27/183682:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357988021213397"/>
+  </r>
+  <r>
+    <n v="878"/>
+    <d v="2010-07-23T13:02:52"/>
+    <x v="5"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.8978299999999999"/>
+    <x v="19"/>
+    <x v="8"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="ERE27"/>
+    <s v="ERE27"/>
+    <x v="16"/>
+    <s v="htc_hero"/>
+    <x v="1"/>
+    <x v="14"/>
+    <s v="chunghwa/htc_hero/hero/hero:2.1-update1/ERE27/183682:user/release-keys"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="357988021213397"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -23185,6 +23845,250 @@
     </format>
   </formats>
   <conditionalFormats count="2">
+    <conditionalFormat priority="1">
+      <pivotAreas count="24">
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="9"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="23"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="2"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="13"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="7"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="15"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="22"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="10"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="16"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="25"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="20"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="6"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="11"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="17"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="24"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="19"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="26"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="8"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="4"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="3"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="21"/>
+            </reference>
+          </references>
+        </pivotArea>
+        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="2">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="20" count="1">
+              <x v="18"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
     <conditionalFormat priority="2">
       <pivotAreas count="24">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
@@ -23613,250 +24517,6 @@
               <x v="3"/>
               <x v="4"/>
               <x v="5"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="18"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </pivotAreas>
-    </conditionalFormat>
-    <conditionalFormat priority="1">
-      <pivotAreas count="24">
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="9"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="23"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="1"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="2"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="13"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="7"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="15"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="22"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="10"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="16"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="25"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="20"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="6"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="11"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="17"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="24"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="19"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="26"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="8"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="4"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="3"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-            <reference field="20" count="1">
-              <x v="21"/>
-            </reference>
-          </references>
-        </pivotArea>
-        <pivotArea type="data" grandCol="1" collapsedLevelsAreSubtotals="1" fieldPosition="0">
-          <references count="2">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
             </reference>
             <reference field="20" count="1">
               <x v="18"/>
@@ -24325,7 +24985,7 @@
   <dimension ref="B2:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -24432,25 +25092,25 @@
         <v>34</v>
       </c>
       <c r="C9" s="6">
-        <v>19.563800000000001</v>
+        <v>20.417250000000003</v>
       </c>
       <c r="D9" s="6">
-        <v>20.592350000000003</v>
+        <v>20.314333333333334</v>
       </c>
       <c r="E9" s="6">
-        <v>29.5059</v>
+        <v>29.591566666666665</v>
       </c>
       <c r="F9" s="6">
-        <v>16.869499999999999</v>
+        <v>16.808974999999997</v>
       </c>
       <c r="G9" s="6">
-        <v>27.144649999999999</v>
+        <v>27.345933333333335</v>
       </c>
       <c r="H9" s="6">
-        <v>25.66375</v>
+        <v>25.632200000000001</v>
       </c>
       <c r="I9" s="15">
-        <v>22.998799999999999</v>
+        <v>23.151249999999997</v>
       </c>
     </row>
     <row r="10" spans="2:9">
@@ -24458,25 +25118,25 @@
         <v>6</v>
       </c>
       <c r="C10" s="6">
-        <v>15.872334285714288</v>
+        <v>15.907547222222226</v>
       </c>
       <c r="D10" s="6">
-        <v>14.462973448275861</v>
+        <v>14.501937666666665</v>
       </c>
       <c r="E10" s="6">
-        <v>18.671042307692304</v>
+        <v>18.689214814814811</v>
       </c>
       <c r="F10" s="6">
-        <v>18.553158571428575</v>
+        <v>18.589053103448279</v>
       </c>
       <c r="G10" s="6">
-        <v>24.065959259259259</v>
+        <v>24.107971428571428</v>
       </c>
       <c r="H10" s="6">
-        <v>22.488084848484849</v>
+        <v>22.388105882352942</v>
       </c>
       <c r="I10" s="15">
-        <v>18.942590842696628</v>
+        <v>18.954565054347821</v>
       </c>
     </row>
     <row r="11" spans="2:9">
@@ -24559,10 +25219,10 @@
         <v>12.491823200000001</v>
       </c>
       <c r="D14" s="6">
-        <v>11.717436153846153</v>
+        <v>11.745934814814813</v>
       </c>
       <c r="E14" s="6">
-        <v>15.669700000000002</v>
+        <v>15.685662500000001</v>
       </c>
       <c r="F14" s="6">
         <v>18.251036842105265</v>
@@ -24571,10 +25231,10 @@
         <v>18.309083999999999</v>
       </c>
       <c r="H14" s="6">
-        <v>18.950385294117641</v>
+        <v>18.984417142857136</v>
       </c>
       <c r="I14" s="15">
-        <v>15.961591578947369</v>
+        <v>15.966729806451616</v>
       </c>
     </row>
     <row r="15" spans="2:9">
@@ -24654,25 +25314,25 @@
         <v>29</v>
       </c>
       <c r="C18" s="6">
-        <v>10.410885454545454</v>
+        <v>10.385745217391305</v>
       </c>
       <c r="D18" s="6">
-        <v>10.320928571428572</v>
+        <v>10.332336363636365</v>
       </c>
       <c r="E18" s="6">
-        <v>16.388391666666667</v>
+        <v>16.313532000000002</v>
       </c>
       <c r="F18" s="6">
-        <v>7.2259175000000013</v>
+        <v>7.2235847619047631</v>
       </c>
       <c r="G18" s="6">
-        <v>14.949708695652173</v>
+        <v>14.895436</v>
       </c>
       <c r="H18" s="6">
-        <v>14.630042307692309</v>
+        <v>14.576396296296297</v>
       </c>
       <c r="I18" s="15">
-        <v>12.557670073529408</v>
+        <v>12.529130909090902</v>
       </c>
     </row>
     <row r="19" spans="2:9">
@@ -24813,22 +25473,22 @@
         <v>5.0388010000000003</v>
       </c>
       <c r="D24" s="6">
-        <v>4.9067046153846148</v>
+        <v>4.8980499999999996</v>
       </c>
       <c r="E24" s="6">
-        <v>6.4911266666666663</v>
+        <v>6.2352729999999994</v>
       </c>
       <c r="F24" s="6">
         <v>7.3704274999999999</v>
       </c>
       <c r="G24" s="6">
-        <v>6.773477777777777</v>
+        <v>6.7621349999999989</v>
       </c>
       <c r="H24" s="6">
-        <v>5.9769220000000001</v>
+        <v>5.9464333333333341</v>
       </c>
       <c r="I24" s="15">
-        <v>5.9710042372881382</v>
+        <v>5.9100532307692326</v>
       </c>
     </row>
     <row r="25" spans="2:9">
@@ -24851,10 +25511,10 @@
         <v>5.7307522222222227</v>
       </c>
       <c r="H25" s="6">
-        <v>4.5478739999999993</v>
+        <v>4.5124054545454539</v>
       </c>
       <c r="I25" s="15">
-        <v>5.0703737735849055</v>
+        <v>5.0534727777777775</v>
       </c>
     </row>
     <row r="26" spans="2:9">
@@ -24874,13 +25534,13 @@
         <v>6.3367260000000005</v>
       </c>
       <c r="G26" s="6">
-        <v>5.9323874999999999</v>
+        <v>6.0004140000000001</v>
       </c>
       <c r="H26" s="6">
         <v>4.7087199999999996</v>
       </c>
       <c r="I26" s="15">
-        <v>4.9736257142857143</v>
+        <v>5.0184151724137926</v>
       </c>
     </row>
     <row r="27" spans="2:9">
@@ -25006,25 +25666,25 @@
         <v>7</v>
       </c>
       <c r="C32" s="8">
-        <v>11.106804429530206</v>
+        <v>11.204981710526321</v>
       </c>
       <c r="D32" s="9">
-        <v>10.357547021126763</v>
+        <v>10.398001804054054</v>
       </c>
       <c r="E32" s="9">
-        <v>15.071068449612401</v>
+        <v>15.131303880597011</v>
       </c>
       <c r="F32" s="9">
-        <v>13.769238842975204</v>
+        <v>13.786099435483873</v>
       </c>
       <c r="G32" s="9">
-        <v>16.157432173913037</v>
+        <v>16.140219513888887</v>
       </c>
       <c r="H32" s="9">
-        <v>16.159537161290316</v>
+        <v>16.039845432098758</v>
       </c>
       <c r="I32" s="13">
-        <v>13.753459432853717</v>
+        <v>13.775207299768519</v>
       </c>
     </row>
     <row r="35" ht="15.75" thickBot="1"/>

</xml_diff>